<commit_message>
S1_TC198-206 and resolve conflict
</commit_message>
<xml_diff>
--- a/Excel Files/Scenario 17/S17_TestCases_Data.xlsx
+++ b/Excel Files/Scenario 17/S17_TestCases_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasin\git\tb-syazwan-ttap-brivge\Excel Files\Scenario 17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasin\OneDrive\Desktop\tb-syazwan-ttap-brivge\Excel Files\Scenario 17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{8197881D-C4E9-4251-A775-1DB8861B7440}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E4AE754E-9534-4EA5-B28C-6223DDAC1BF8}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="63" firstSheet="61" tabRatio="567" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView activeTab="54" firstSheet="54" tabRatio="567" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="AutoIncrement" r:id="rId1" sheetId="86"/>
@@ -30,56 +30,57 @@
     <sheet name="TC9- Contract List" r:id="rId15" sheetId="17"/>
     <sheet name="TC10- Parts List" r:id="rId16" sheetId="55"/>
     <sheet name="T11- RequestNo" r:id="rId17" sheetId="77"/>
-    <sheet name="TC16- New Firm Qty" r:id="rId18" sheetId="18"/>
-    <sheet name="TC16- New Inbound Date1" r:id="rId19" sheetId="35"/>
-    <sheet name="TC17- Regular Customer No" r:id="rId20" sheetId="79"/>
-    <sheet name="TC19-Delivery Plan" r:id="rId21" sheetId="37"/>
-    <sheet name="TC19- Order Price" r:id="rId22" sheetId="36"/>
-    <sheet name="TC19- Sales Order No" r:id="rId23" sheetId="80"/>
-    <sheet name="TC21- Forecast Change" r:id="rId24" sheetId="34"/>
-    <sheet name="TC21- RequestNo" r:id="rId25" sheetId="56"/>
-    <sheet name="TC22- Parts Detail" r:id="rId26" sheetId="38"/>
-    <sheet name="TC26- Parts Detail" r:id="rId27" sheetId="57"/>
-    <sheet name="TC27-Change Firm Qty" r:id="rId28" sheetId="21"/>
-    <sheet name=" T27- Change Inbound Date" r:id="rId29" sheetId="23"/>
-    <sheet name="TC27- Request No" r:id="rId30" sheetId="88"/>
-    <sheet name="TC28- Parts Detail" r:id="rId31" sheetId="89"/>
-    <sheet name="T31-Parts Detail" r:id="rId32" sheetId="90"/>
-    <sheet name="TC32- Sales Order Info" r:id="rId33" sheetId="25"/>
-    <sheet name="TC33- Customer Forecast Detail" r:id="rId34" sheetId="26"/>
-    <sheet name="TC34- Request No" r:id="rId35" sheetId="91"/>
-    <sheet name="T35- Parts Detail" r:id="rId36" sheetId="28"/>
-    <sheet name="TC38- Change Firm Qty" r:id="rId37" sheetId="31"/>
-    <sheet name="TC40- Units Part Master" r:id="rId38" sheetId="33"/>
-    <sheet name="TC41- Temp Firm Quantity" r:id="rId39" sheetId="41"/>
-    <sheet name="TC41.1-Temp Outbound Date" r:id="rId40" sheetId="42"/>
-    <sheet name="TC42- Edit Firm Quantity1" r:id="rId41" sheetId="45"/>
-    <sheet name="TC42- Request No" r:id="rId42" sheetId="92"/>
-    <sheet name="TC43- Parts Detail" r:id="rId43" sheetId="47"/>
-    <sheet name="TC46- Parts Detail" r:id="rId44" sheetId="48"/>
-    <sheet name="TC50- Request No" r:id="rId45" sheetId="93"/>
-    <sheet name="TC51- Outbound Details" r:id="rId46" sheetId="49"/>
-    <sheet name="TC54-Purchase Amount By Sup" r:id="rId47" sheetId="81"/>
-    <sheet name="TC55- Complete Deliveries List" r:id="rId48" sheetId="82"/>
-    <sheet name="TC55- New Firm Quantity" r:id="rId49" sheetId="52"/>
-    <sheet name="TC55- New Outbound Date" r:id="rId50" sheetId="53"/>
-    <sheet name="TC55- Request No" r:id="rId51" sheetId="94"/>
-    <sheet name="TC56- Part Details" r:id="rId52" sheetId="54"/>
-    <sheet name="TC60- Parts Detail1" r:id="rId53" sheetId="59"/>
-    <sheet name="TC63- New Firm Quantity" r:id="rId54" sheetId="60"/>
-    <sheet name="TC63- New Oubound Date" r:id="rId55" sheetId="61"/>
-    <sheet name="TC63- Request No" r:id="rId56" sheetId="95"/>
-    <sheet name="TC69- Outbound Details" r:id="rId57" sheetId="62"/>
-    <sheet name="TC71 &amp; 72- CargoTrackingDetail " r:id="rId58" sheetId="63"/>
-    <sheet name="T73- Shipping Detail" r:id="rId59" sheetId="67"/>
-    <sheet name="TC75- Customer Inbound Details" r:id="rId60" sheetId="69"/>
-    <sheet name="TC75- Outbound Nos" r:id="rId61" sheetId="71"/>
-    <sheet name="TC76- Purchase Amount By Sup" r:id="rId62" sheetId="84"/>
-    <sheet name="TC76- Complete Deliveries List" r:id="rId63" sheetId="85"/>
-    <sheet name="TC78 - Supplier SellerGIInvoice" r:id="rId64" sheetId="72"/>
+    <sheet name="TC16- Tenth Day Period" r:id="rId18" sheetId="96"/>
+    <sheet name="TC16- New Firm Qty" r:id="rId19" sheetId="18"/>
+    <sheet name="TC16- New Inbound Date1" r:id="rId20" sheetId="35"/>
+    <sheet name="TC17- Regular Customer No" r:id="rId21" sheetId="79"/>
+    <sheet name="TC19-Delivery Plan" r:id="rId22" sheetId="37"/>
+    <sheet name="TC19- Order Price" r:id="rId23" sheetId="36"/>
+    <sheet name="TC19- Sales Order No" r:id="rId24" sheetId="80"/>
+    <sheet name="TC21- Forecast Change" r:id="rId25" sheetId="34"/>
+    <sheet name="TC21- RequestNo" r:id="rId26" sheetId="56"/>
+    <sheet name="TC22- Parts Detail" r:id="rId27" sheetId="38"/>
+    <sheet name="TC26- Parts Detail" r:id="rId28" sheetId="57"/>
+    <sheet name="TC27-Change Firm Qty" r:id="rId29" sheetId="21"/>
+    <sheet name=" T27- Change Inbound Date" r:id="rId30" sheetId="23"/>
+    <sheet name="TC27- Request No" r:id="rId31" sheetId="88"/>
+    <sheet name="TC28- Parts Detail" r:id="rId32" sheetId="89"/>
+    <sheet name="T31-Parts Detail" r:id="rId33" sheetId="90"/>
+    <sheet name="TC32- Sales Order Info" r:id="rId34" sheetId="25"/>
+    <sheet name="TC33- Customer Forecast Detail" r:id="rId35" sheetId="26"/>
+    <sheet name="TC34- Request No" r:id="rId36" sheetId="91"/>
+    <sheet name="T35- Parts Detail" r:id="rId37" sheetId="28"/>
+    <sheet name="TC38- Change Firm Qty" r:id="rId38" sheetId="31"/>
+    <sheet name="TC40- Units Part Master" r:id="rId39" sheetId="33"/>
+    <sheet name="TC41- Temp Firm Quantity" r:id="rId40" sheetId="41"/>
+    <sheet name="TC41.1-Temp Outbound Date" r:id="rId41" sheetId="42"/>
+    <sheet name="TC42- Edit Firm Quantity1" r:id="rId42" sheetId="45"/>
+    <sheet name="TC42- Request No" r:id="rId43" sheetId="92"/>
+    <sheet name="TC43- Parts Detail" r:id="rId44" sheetId="47"/>
+    <sheet name="TC46- Parts Detail" r:id="rId45" sheetId="48"/>
+    <sheet name="TC50- Request No" r:id="rId46" sheetId="93"/>
+    <sheet name="TC51- Outbound Details" r:id="rId47" sheetId="49"/>
+    <sheet name="TC54-Purchase Amount By Sup" r:id="rId48" sheetId="81"/>
+    <sheet name="TC55- Complete Deliveries List" r:id="rId49" sheetId="82"/>
+    <sheet name="TC55- New Firm Quantity" r:id="rId50" sheetId="52"/>
+    <sheet name="TC55- New Outbound Date" r:id="rId51" sheetId="53"/>
+    <sheet name="TC55- Request No" r:id="rId52" sheetId="94"/>
+    <sheet name="TC56- Part Details" r:id="rId53" sheetId="54"/>
+    <sheet name="TC60- Parts Detail1" r:id="rId54" sheetId="59"/>
+    <sheet name="TC63- New Firm Quantity" r:id="rId55" sheetId="60"/>
+    <sheet name="TC63- New Oubound Date" r:id="rId56" sheetId="61"/>
+    <sheet name="TC63- Request No" r:id="rId57" sheetId="95"/>
+    <sheet name="TC69- Outbound Details" r:id="rId58" sheetId="62"/>
+    <sheet name="TC71 &amp; 72- CargoTrackingDetail " r:id="rId59" sheetId="63"/>
+    <sheet name="T73- Shipping Detail" r:id="rId60" sheetId="67"/>
+    <sheet name="TC75- Customer Inbound Details" r:id="rId61" sheetId="69"/>
+    <sheet name="TC75- Outbound Nos" r:id="rId62" sheetId="71"/>
+    <sheet name="TC76- Purchase Amount By Sup" r:id="rId63" sheetId="84"/>
+    <sheet name="TC76- Complete Deliveries List" r:id="rId64" sheetId="85"/>
+    <sheet name="TC78 - Supplier SellerGIInvoice" r:id="rId65" sheetId="72"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId65"/>
+    <externalReference r:id="rId66"/>
   </externalReferences>
   <definedNames>
     <definedName name="UOM">[1]UOM!$A$1:$A$36</definedName>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="370">
   <si>
     <t>NEW/MOD</t>
   </si>
@@ -675,9 +676,6 @@
     <t>InboundDate2</t>
   </si>
   <si>
-    <t>New Forecast_N+1</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
@@ -1134,9 +1132,6 @@
     <t>Please set eration</t>
   </si>
   <si>
-    <t>b00005</t>
-  </si>
-  <si>
     <t>Inbound_plan_4</t>
   </si>
   <si>
@@ -1155,46 +1150,61 @@
     <t>Old_outbound_Supplier_4</t>
   </si>
   <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>CR-PK-CUS-POC-2310038</t>
-  </si>
-  <si>
-    <t>R-PK-CUS-POC-2310072</t>
-  </si>
-  <si>
-    <t>R-PK-CUS-POC-2310073</t>
-  </si>
-  <si>
-    <t>R-PK-CUS-POC-2310074</t>
-  </si>
-  <si>
-    <t>cs1702-2310001</t>
-  </si>
-  <si>
-    <t>ss1702-2310001</t>
-  </si>
-  <si>
-    <t>R-PK-CUS-POC-2310076</t>
-  </si>
-  <si>
-    <t>o-PK-SUP-POC-231024001</t>
-  </si>
-  <si>
-    <t>o-PK-SUP-POC-231024002</t>
-  </si>
-  <si>
-    <t>o-PK-SUP-POC-231024003</t>
-  </si>
-  <si>
-    <t>PKS2310031</t>
-  </si>
-  <si>
-    <t>PKS2310032</t>
-  </si>
-  <si>
-    <t>PKS2310033</t>
+    <t>Auto Generate Tenth Day Period</t>
+  </si>
+  <si>
+    <t>o-PK-SUP-POC-231029009</t>
+  </si>
+  <si>
+    <t>PKS2310068</t>
+  </si>
+  <si>
+    <t>PKS2310069</t>
+  </si>
+  <si>
+    <t>PKS2310070</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>R-PK-CUS-POC-2310209</t>
+  </si>
+  <si>
+    <t>CR-PK-CUS-POC-2310081</t>
+  </si>
+  <si>
+    <t>R-PK-CUS-POC-2310210</t>
+  </si>
+  <si>
+    <t>R-PK-CUS-POC-2310211</t>
+  </si>
+  <si>
+    <t>cs1731-2310001</t>
+  </si>
+  <si>
+    <t>ss1731-2310001</t>
+  </si>
+  <si>
+    <t>R-PK-CUS-POC-2310212</t>
+  </si>
+  <si>
+    <t>o-PK-SUP-POC-231030001</t>
+  </si>
+  <si>
+    <t>o-PK-SUP-POC-231030002</t>
+  </si>
+  <si>
+    <t>o-PK-SUP-POC-231031001</t>
+  </si>
+  <si>
+    <t>PKS2310071</t>
+  </si>
+  <si>
+    <t>PKS2310072</t>
+  </si>
+  <si>
+    <t>PKS2310073</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1221,7 @@
     <numFmt numFmtId="169" formatCode="0.000000"/>
     <numFmt numFmtId="170" formatCode="mmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1267,6 +1277,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF343541"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1387,7 +1409,7 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
@@ -1496,6 +1518,8 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="10" numFmtId="15" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle builtinId="3" name="Comma" xfId="2"/>
@@ -1984,7 +2008,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1995,17 +2019,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="54" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
@@ -2073,7 +2097,7 @@
       </c>
       <c r="D2" t="str">
         <f>'TC2- Contract Parts Info'!D2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E2" t="s">
         <v>100</v>
@@ -2082,7 +2106,7 @@
         <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2097,7 +2121,7 @@
       </c>
       <c r="D3" t="str">
         <f>'TC2- Contract Parts Info'!D3</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E3" t="s">
         <v>100</v>
@@ -2106,7 +2130,7 @@
         <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2121,7 +2145,7 @@
       </c>
       <c r="D4" t="str">
         <f>'TC2- Contract Parts Info'!D4</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E4" t="s">
         <v>100</v>
@@ -2130,7 +2154,7 @@
         <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2145,7 +2169,7 @@
       </c>
       <c r="D5" t="str">
         <f>'TC2- Contract Parts Info'!D5</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E5" t="s">
         <v>100</v>
@@ -2154,7 +2178,7 @@
         <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2168,23 +2192,23 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="23.5546875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="19.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -2197,7 +2221,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A28" sqref="A27:A28"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2327,7 +2351,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -2371,7 +2395,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="B2" s="25">
         <v>1</v>
@@ -2424,7 +2448,7 @@
         <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -2436,34 +2460,34 @@
         <v>93</v>
       </c>
       <c r="H1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I1" t="s">
         <v>305</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>306</v>
       </c>
-      <c r="J1" t="s">
-        <v>307</v>
-      </c>
       <c r="K1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L1" t="s">
+        <v>308</v>
+      </c>
+      <c r="M1" t="s">
         <v>309</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>310</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>311</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>312</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>313</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>314</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
@@ -2472,7 +2496,7 @@
         <v>20</v>
       </c>
       <c r="T1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U1" t="s">
         <v>95</v>
@@ -2484,13 +2508,13 @@
         <v>21</v>
       </c>
       <c r="X1" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y1" t="s">
         <v>316</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>317</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>318</v>
       </c>
       <c r="AA1" t="s">
         <v>22</v>
@@ -2532,7 +2556,7 @@
       </c>
       <c r="J2" t="str">
         <f ca="1">TEXT(TODAY(), "mmm d, yyyy")</f>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R2">
         <v>10</v>
@@ -2601,7 +2625,7 @@
       </c>
       <c r="J3" t="str">
         <f ca="1" ref="J3:J6" si="0" t="shared">TEXT(TODAY(), "mmm d, yyyy")</f>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R3">
         <v>10</v>
@@ -2670,7 +2694,7 @@
       </c>
       <c r="J4" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R4">
         <v>10</v>
@@ -2739,7 +2763,7 @@
       </c>
       <c r="J5" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R5">
         <v>10</v>
@@ -2808,7 +2832,7 @@
       </c>
       <c r="J6" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R6">
         <v>10</v>
@@ -2904,7 +2928,7 @@
       </c>
       <c r="D2" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E2" t="s">
         <v>100</v>
@@ -2913,7 +2937,7 @@
         <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2928,7 +2952,7 @@
       </c>
       <c r="D3" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E3" t="s">
         <v>100</v>
@@ -2937,7 +2961,7 @@
         <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2952,7 +2976,7 @@
       </c>
       <c r="D4" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E4" t="s">
         <v>100</v>
@@ -2961,7 +2985,7 @@
         <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2976,7 +3000,7 @@
       </c>
       <c r="D5" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E5" t="s">
         <v>100</v>
@@ -2985,7 +3009,7 @@
         <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3000,7 +3024,7 @@
       </c>
       <c r="D6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E6" t="s">
         <v>100</v>
@@ -3009,7 +3033,7 @@
         <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -3043,10 +3067,10 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$K$2</f>
-        <v>s1702</v>
+        <v>s1731</v>
       </c>
       <c r="B2" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3055,6 +3079,35 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F8C9AC-BFC1-4F74-A888-81960B4CD9E6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="29.44140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="15" r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row ht="15" r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="56" t="str">
+        <f ca="1">TEXT(DATE(YEAR(TODAY()), 10, 22)+((INT((TODAY()-DATE(YEAR(TODAY()),10,21))/10))*10),"mmm d, yyyy") &amp; " ~ " &amp; TEXT(DATE(YEAR(TODAY()), 10, 31)+((INT((TODAY()-DATE(YEAR(TODAY()),10,21))/10))*10),"mmm d, yyyy")</f>
+        <v>Nov 1, 2023 ~ Nov 10, 2023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EB5BCC-E864-435B-857D-D35862E35EB0}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -3163,40 +3216,6 @@
       </c>
       <c r="E6">
         <v>600</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A15540F-447C-472A-9FC9-ECC8F627E6F5}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" customWidth="true" width="35.88671875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
-        <v>45240</v>
-      </c>
-      <c r="B2" s="30">
-        <v>45250</v>
       </c>
     </row>
   </sheetData>
@@ -3494,6 +3513,40 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A15540F-447C-472A-9FC9-ECC8F627E6F5}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" customWidth="true" width="35.88671875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="30">
+        <v>45270</v>
+      </c>
+      <c r="B2" s="30">
+        <v>45280</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEDC36B2-2345-4809-9DF4-82A2306D2076}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3510,12 +3563,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3523,7 +3576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01064E38-B985-4C88-953C-91312F7E645E}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -3581,7 +3634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688A99D8-A546-4793-BF80-17BCE9AC2E6A}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -3607,7 +3660,7 @@
         <v>9.01</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3615,7 +3668,7 @@
         <v>7.01</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3623,7 +3676,7 @@
         <v>10.01</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3631,7 +3684,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3639,7 +3692,7 @@
         <v>100.68</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3647,12 +3700,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F8BF62-0F7A-4A26-AEBF-44DCC1217B1A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I27" sqref="I26:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3663,60 +3716,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E387D73C-C5A5-49CC-84DA-30FD52F9787C}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="27.5546875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33">
-        <v>1000</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3725,11 +3730,96 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E387D73C-C5A5-49CC-84DA-30FD52F9787C}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.5546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="33">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="33">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C93116F-C081-465D-B251-5D5DDE8C10B4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3745,8 +3835,8 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
-        <f>"r"&amp;'TC17- Regular Customer No'!$A$2&amp;"-"&amp;"02"</f>
-        <v>rcs1702-2310001-02</v>
+        <f>"r"&amp;'TC17- Regular Customer No'!$A$2&amp;"-"&amp;"01"</f>
+        <v>rcs1731-2310001-01</v>
       </c>
     </row>
   </sheetData>
@@ -3754,12 +3844,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8295D9FD-18AA-4414-88C1-5A2C28BBBFD0}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3778,10 +3868,10 @@
         <v>124</v>
       </c>
       <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
         <v>195</v>
-      </c>
-      <c r="C1" t="s">
-        <v>196</v>
       </c>
       <c r="D1" t="s">
         <v>144</v>
@@ -3805,10 +3895,10 @@
         <v>102</v>
       </c>
       <c r="K1" t="s">
+        <v>251</v>
+      </c>
+      <c r="L1" t="s">
         <v>252</v>
-      </c>
-      <c r="L1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -3887,12 +3977,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA8620A-4A8E-4AAE-B2CE-F0EEF0338C09}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3907,10 +3997,10 @@
         <v>124</v>
       </c>
       <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
         <v>195</v>
-      </c>
-      <c r="C1" t="s">
-        <v>196</v>
       </c>
       <c r="D1" t="s">
         <v>144</v>
@@ -3934,30 +4024,30 @@
         <v>102</v>
       </c>
       <c r="K1" t="s">
+        <v>251</v>
+      </c>
+      <c r="L1" t="s">
         <v>252</v>
-      </c>
-      <c r="L1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -3966,33 +4056,33 @@
         <v>10</v>
       </c>
       <c r="J2" s="32">
+        <v>800</v>
+      </c>
+      <c r="K2" s="32">
+        <v>800</v>
+      </c>
+      <c r="L2" s="32">
         <v>1000</v>
-      </c>
-      <c r="K2" s="32">
-        <v>1000</v>
-      </c>
-      <c r="L2" s="32">
-        <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -4001,48 +4091,13 @@
         <v>10</v>
       </c>
       <c r="J3" s="32">
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="K3" s="32">
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="L3" s="32">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4" s="32">
-        <v>1600</v>
-      </c>
-      <c r="K4" s="32">
-        <v>1600</v>
-      </c>
-      <c r="L4" s="32">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
@@ -4050,12 +4105,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAA4611-B951-475F-8E0F-A612CCEB920F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4175,12 +4230,41 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2023D2A2-A733-426A-8565-677FAAC3BE3A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="19.6640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>'TC2- ReceivedRequestAddNewPart'!$K$2</f>
+        <v>s1731</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398FF2F2-BB87-4EBD-BB67-BC80830F281F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B27:B28"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4201,13 +4285,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="30">
-        <v>45240</v>
+        <v>45270</v>
       </c>
       <c r="B2" s="30">
-        <v>45245</v>
+        <v>45280</v>
       </c>
       <c r="C2" s="30">
-        <v>45270</v>
+        <v>45301</v>
       </c>
     </row>
   </sheetData>
@@ -4215,41 +4299,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2023D2A2-A733-426A-8565-677FAAC3BE3A}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="19.6640625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f>'TC2- ReceivedRequestAddNewPart'!$K$2</f>
-        <v>s1702</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E643A149-B87E-4DD7-A3D9-F8B3E4DB4447}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4264,8 +4319,8 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
-        <f>'TC21- RequestNo'!$A$2</f>
-        <v>rcs1702-2310001-02</v>
+        <f>"r"&amp;'TC17- Regular Customer No'!$A$2&amp;"-"&amp;"02"</f>
+        <v>rcs1731-2310001-02</v>
       </c>
     </row>
   </sheetData>
@@ -4273,12 +4328,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43AE63B-7AAE-42E4-89C6-4F58557162BE}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4293,22 +4348,20 @@
     <col min="12" max="12" customWidth="true" width="17.21875" collapsed="true"/>
     <col min="13" max="13" customWidth="true" width="12.0" collapsed="true"/>
     <col min="14" max="14" customWidth="true" width="18.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="15.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>124</v>
       </c>
       <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
         <v>195</v>
-      </c>
-      <c r="C1" t="s">
-        <v>196</v>
       </c>
       <c r="D1" t="s">
         <v>144</v>
@@ -4347,19 +4400,13 @@
         <v>152</v>
       </c>
       <c r="P1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="Q1" t="s">
-        <v>154</v>
-      </c>
-      <c r="R1" t="s">
-        <v>155</v>
-      </c>
-      <c r="S1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -4393,17 +4440,17 @@
       <c r="M2" t="s">
         <v>157</v>
       </c>
+      <c r="O2" s="32">
+        <v>800</v>
+      </c>
       <c r="P2" s="32">
         <v>800</v>
       </c>
-      <c r="R2" s="32">
-        <v>800</v>
-      </c>
-      <c r="S2">
+      <c r="Q2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -4437,55 +4484,11 @@
       <c r="M3" t="s">
         <v>157</v>
       </c>
+      <c r="O3" s="32">
+        <v>1600</v>
+      </c>
       <c r="P3" s="32">
-        <v>1600</v>
-      </c>
-      <c r="R3" s="32">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4" s="32">
-        <v>1000</v>
-      </c>
-      <c r="K4" s="32">
-        <v>1000</v>
-      </c>
-      <c r="M4" t="s">
-        <v>157</v>
-      </c>
-      <c r="O4">
-        <v>400</v>
-      </c>
-      <c r="P4">
-        <v>600</v>
-      </c>
-      <c r="Q4">
-        <v>400</v>
-      </c>
-      <c r="R4">
-        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -4494,12 +4497,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BE52D5-E46D-41A4-A6A6-4DDA1680687F}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4519,7 +4522,7 @@
         <v>186</v>
       </c>
       <c r="C1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D1" t="s">
         <v>145</v>
@@ -4645,47 +4648,6 @@
       <c r="P3" s="32"/>
       <c r="Q3" s="32">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4" s="32">
-        <v>1000</v>
-      </c>
-      <c r="J4" s="32">
-        <v>1500</v>
-      </c>
-      <c r="L4" t="s">
-        <v>157</v>
-      </c>
-      <c r="N4">
-        <v>400</v>
-      </c>
-      <c r="O4">
-        <v>600</v>
-      </c>
-      <c r="P4">
-        <v>400</v>
-      </c>
-      <c r="Q4">
-        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -4693,7 +4655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA77A46-DDE3-43E3-B541-11491347B436}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
@@ -4775,10 +4737,10 @@
         <v>174</v>
       </c>
       <c r="U1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="V1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W1" t="s">
         <v>175</v>
@@ -4790,7 +4752,7 @@
         <v>177</v>
       </c>
       <c r="Z1" s="29" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -4805,7 +4767,7 @@
       </c>
       <c r="D2" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1702-2310001</v>
+        <v>cs1731-2310001</v>
       </c>
       <c r="E2" t="s">
         <v>72</v>
@@ -4823,7 +4785,7 @@
         <v>9.01</v>
       </c>
       <c r="J2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K2" t="s">
         <v>178</v>
@@ -4886,7 +4848,7 @@
       </c>
       <c r="D3" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1702-2310001</v>
+        <v>cs1731-2310001</v>
       </c>
       <c r="E3" t="s">
         <v>72</v>
@@ -4904,7 +4866,7 @@
         <v>7.01</v>
       </c>
       <c r="J3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K3" t="s">
         <v>178</v>
@@ -4967,7 +4929,7 @@
       </c>
       <c r="D4" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1702-2310001</v>
+        <v>cs1731-2310001</v>
       </c>
       <c r="E4" t="s">
         <v>72</v>
@@ -4985,7 +4947,7 @@
         <v>10.01</v>
       </c>
       <c r="J4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K4" t="s">
         <v>178</v>
@@ -5048,7 +5010,7 @@
       </c>
       <c r="D5" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1702-2310001</v>
+        <v>cs1731-2310001</v>
       </c>
       <c r="E5" t="s">
         <v>72</v>
@@ -5066,7 +5028,7 @@
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K5" t="s">
         <v>178</v>
@@ -5129,7 +5091,7 @@
       </c>
       <c r="D6" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1702-2310001</v>
+        <v>cs1731-2310001</v>
       </c>
       <c r="E6" t="s">
         <v>72</v>
@@ -5147,7 +5109,7 @@
         <v>100.68</v>
       </c>
       <c r="J6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K6" t="s">
         <v>178</v>
@@ -5204,12 +5166,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C097B8-9E0B-4919-8936-C8FA44A90F17}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D19" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5257,7 +5219,7 @@
       </c>
       <c r="D2" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="E2" t="s">
         <v>71</v>
@@ -5284,7 +5246,7 @@
       </c>
       <c r="D3" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="E3" t="s">
         <v>71</v>
@@ -5311,7 +5273,7 @@
       </c>
       <c r="D4" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
@@ -5338,7 +5300,7 @@
       </c>
       <c r="D5" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="E5" t="s">
         <v>71</v>
@@ -5365,7 +5327,7 @@
       </c>
       <c r="D6" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="E6" t="s">
         <v>71</v>
@@ -5386,12 +5348,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4060209A-0B38-4661-9596-27A202D9FCC3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5407,7 +5369,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>"r"&amp;'TC19- Sales Order No'!$A$2&amp;"-01"</f>
-        <v>rss1702-2310001-01</v>
+        <v>rss1731-2310001-01</v>
       </c>
     </row>
   </sheetData>
@@ -5415,7 +5377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81805742-040D-4C75-AD7F-AC26A3786CA2}">
   <dimension ref="A1:V6"/>
   <sheetViews>
@@ -5474,28 +5436,28 @@
         <v>151</v>
       </c>
       <c r="N1" t="s">
+        <v>201</v>
+      </c>
+      <c r="O1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" t="s">
         <v>202</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>348</v>
+      </c>
+      <c r="R1" t="s">
         <v>204</v>
       </c>
-      <c r="P1" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>350</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>206</v>
+      </c>
+      <c r="T1" t="s">
+        <v>207</v>
+      </c>
+      <c r="U1" t="s">
         <v>205</v>
-      </c>
-      <c r="S1" t="s">
-        <v>207</v>
-      </c>
-      <c r="T1" t="s">
-        <v>208</v>
-      </c>
-      <c r="U1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -5732,13 +5694,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93B6DC3-11C4-484A-99A7-37E57C28C17F}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5833,12 +5793,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5330B2FD-88D7-4407-ACFA-FC66B38BF634}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5901,134 +5861,6 @@
       <c r="C5" s="35" t="s">
         <v>39</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA414E7-A38B-4919-8C8F-D39CE665F9A5}">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="12.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.77734375" collapsed="true"/>
-    <col min="4" max="7" customWidth="true" width="29.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.77734375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="31">
-        <v>800</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31">
-        <v>800</v>
-      </c>
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="31">
-        <v>1200</v>
-      </c>
-      <c r="D3" s="31">
-        <v>500</v>
-      </c>
-      <c r="E3" s="31">
-        <v>700</v>
-      </c>
-      <c r="F3" s="31"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="31">
-        <v>900</v>
-      </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31">
-        <v>800</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="31">
-        <v>1500</v>
-      </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="31">
-        <v>0</v>
-      </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -6081,11 +5913,11 @@
       </c>
       <c r="B2" t="str">
         <f>"Sc17"&amp;"-"&amp;AutoIncrement!A2&amp;" "&amp;"Free"</f>
-        <v>Sc17-02 Free</v>
+        <v>Sc17-31 Free</v>
       </c>
       <c r="C2" t="str">
         <f>"Sc17"&amp;"-"&amp;AutoIncrement!A2&amp;" "&amp;"Free"&amp;"- 30 Days"</f>
-        <v>Sc17-02 Free- 30 Days</v>
+        <v>Sc17-31 Free- 30 Days</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -6106,11 +5938,139 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA414E7-A38B-4919-8C8F-D39CE665F9A5}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="4" max="7" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.77734375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="31">
+        <v>800</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31">
+        <v>800</v>
+      </c>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="31">
+        <v>1200</v>
+      </c>
+      <c r="D3" s="31">
+        <v>500</v>
+      </c>
+      <c r="E3" s="31">
+        <v>700</v>
+      </c>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="31">
+        <v>900</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31">
+        <v>800</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="31">
+        <v>1500</v>
+      </c>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="31">
+        <v>0</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0E1383-5F8F-418A-8F6C-BD1F737AB025}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6121,30 +6081,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>200</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="41">
-        <v>45235</v>
+        <v>45265</v>
       </c>
       <c r="B2" s="41">
-        <v>45240</v>
+        <v>45270</v>
       </c>
       <c r="C2" s="41">
-        <v>45243</v>
+        <v>45273</v>
       </c>
       <c r="D2" s="40">
-        <v>45270</v>
+        <v>45292</v>
       </c>
     </row>
   </sheetData>
@@ -6152,12 +6112,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC55F55F-CBAA-44C1-8C2F-96B3D03911C9}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6185,7 +6145,7 @@
         <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -6276,12 +6236,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1350DA43-153F-4D15-8B00-E8BA26878F38}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6291,13 +6251,13 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
-        <f>'TC63- Request No'!A2</f>
-        <v>rss1702-2310001-04</v>
+        <f>"r"&amp;'TC19- Sales Order No'!$A$2&amp;"-02"</f>
+        <v>rss1731-2310001-02</v>
       </c>
     </row>
   </sheetData>
@@ -6305,7 +6265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2925DC33-A3BF-4DC0-9998-0A8ED380A76F}">
   <dimension ref="A1:V6"/>
   <sheetViews>
@@ -6359,28 +6319,28 @@
         <v>151</v>
       </c>
       <c r="N1" t="s">
+        <v>201</v>
+      </c>
+      <c r="O1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" t="s">
         <v>202</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>348</v>
+      </c>
+      <c r="R1" t="s">
         <v>204</v>
       </c>
-      <c r="P1" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>350</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>206</v>
+      </c>
+      <c r="T1" t="s">
+        <v>207</v>
+      </c>
+      <c r="U1" t="s">
         <v>205</v>
-      </c>
-      <c r="S1" t="s">
-        <v>207</v>
-      </c>
-      <c r="T1" t="s">
-        <v>208</v>
-      </c>
-      <c r="U1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -6613,7 +6573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0818C847-4211-4653-8825-BBEEDE381DD7}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -6636,7 +6596,7 @@
         <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
         <v>182</v>
@@ -6675,46 +6635,46 @@
         <v>151</v>
       </c>
       <c r="O1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P1" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q1" t="s">
         <v>202</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>204</v>
       </c>
-      <c r="Q1" t="s">
-        <v>203</v>
-      </c>
-      <c r="R1" t="s">
-        <v>205</v>
-      </c>
       <c r="S1" t="s">
+        <v>206</v>
+      </c>
+      <c r="T1" t="s">
         <v>207</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>208</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>209</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>210</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
+        <v>350</v>
+      </c>
+      <c r="Y1" t="s">
         <v>211</v>
       </c>
-      <c r="X1" t="s">
-        <v>352</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>212</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>213</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>214</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -6997,7 +6957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6FE45A-8ADD-4DCB-AC8A-544D349118A6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -7017,7 +6977,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -7025,12 +6985,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60525806-95C1-4FC3-A8EC-C8D201E4ADF4}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7053,79 +7013,79 @@
         <v>99</v>
       </c>
       <c r="B1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" t="s">
         <v>216</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>217</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>218</v>
       </c>
-      <c r="E1" t="s">
-        <v>219</v>
-      </c>
       <c r="F1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" t="s">
         <v>221</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>222</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>223</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>224</v>
-      </c>
-      <c r="J1" t="s">
-        <v>225</v>
       </c>
       <c r="K1" t="s">
         <v>128</v>
       </c>
       <c r="L1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N1" t="s">
+        <v>231</v>
+      </c>
+      <c r="O1" t="s">
         <v>232</v>
-      </c>
-      <c r="O1" t="s">
-        <v>233</v>
       </c>
       <c r="P1" t="s">
         <v>21</v>
       </c>
       <c r="Q1" t="s">
+        <v>233</v>
+      </c>
+      <c r="R1" t="s">
         <v>234</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>235</v>
       </c>
-      <c r="S1" t="s">
-        <v>236</v>
-      </c>
       <c r="T1" t="s">
+        <v>242</v>
+      </c>
+      <c r="U1" t="s">
         <v>243</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>244</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>245</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>246</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>247</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>248</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -7137,13 +7097,14 @@
       </c>
       <c r="C2" t="str">
         <f>"o-PK-SUP-POC-230720001-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720001-02</v>
+        <v>o-PK-SUP-POC-230720001-31</v>
       </c>
       <c r="D2" s="30">
         <v>45218</v>
       </c>
-      <c r="E2" t="s">
-        <v>220</v>
+      <c r="E2" t="str">
+        <f>"B-230720001-"&amp;AutoIncrement!A2</f>
+        <v>B-230720001-31</v>
       </c>
       <c r="F2" t="s">
         <v>80</v>
@@ -7158,7 +7119,7 @@
         <v>69</v>
       </c>
       <c r="J2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K2" t="s">
         <v>72</v>
@@ -7167,13 +7128,13 @@
         <v>72</v>
       </c>
       <c r="M2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N2" t="s">
+        <v>236</v>
+      </c>
+      <c r="O2" t="s">
         <v>237</v>
-      </c>
-      <c r="O2" t="s">
-        <v>238</v>
       </c>
       <c r="P2">
         <v>100.01</v>
@@ -7185,11 +7146,11 @@
         <v>100.01</v>
       </c>
       <c r="S2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="T2" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="U2" t="s">
         <v>71</v>
@@ -7219,13 +7180,14 @@
       </c>
       <c r="C3" t="str">
         <f>"o-PK-SUP-POC-230720001-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720001-02</v>
+        <v>o-PK-SUP-POC-230720001-31</v>
       </c>
       <c r="D3" s="30">
         <v>45218</v>
       </c>
-      <c r="E3" t="s">
-        <v>220</v>
+      <c r="E3" t="str">
+        <f>"B-230720001-"&amp;AutoIncrement!A2</f>
+        <v>B-230720001-31</v>
       </c>
       <c r="F3" t="s">
         <v>83</v>
@@ -7240,7 +7202,7 @@
         <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K3" t="s">
         <v>72</v>
@@ -7249,13 +7211,13 @@
         <v>72</v>
       </c>
       <c r="M3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O3" t="s">
         <v>240</v>
-      </c>
-      <c r="O3" t="s">
-        <v>241</v>
       </c>
       <c r="P3">
         <v>100.01</v>
@@ -7267,11 +7229,11 @@
         <v>100.01</v>
       </c>
       <c r="S3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="T3" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="U3" t="s">
         <v>71</v>
@@ -7301,13 +7263,14 @@
       </c>
       <c r="C4" t="str">
         <f>"o-PK-SUP-POC-230720001-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720001-02</v>
+        <v>o-PK-SUP-POC-230720001-31</v>
       </c>
       <c r="D4" s="30">
         <v>45218</v>
       </c>
-      <c r="E4" t="s">
-        <v>220</v>
+      <c r="E4" t="str">
+        <f>"B-230720001-"&amp;AutoIncrement!A2</f>
+        <v>B-230720001-31</v>
       </c>
       <c r="F4" t="s">
         <v>85</v>
@@ -7322,7 +7285,7 @@
         <v>69</v>
       </c>
       <c r="J4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K4" t="s">
         <v>72</v>
@@ -7331,13 +7294,13 @@
         <v>72</v>
       </c>
       <c r="M4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N4" t="s">
+        <v>236</v>
+      </c>
+      <c r="O4" t="s">
         <v>237</v>
-      </c>
-      <c r="O4" t="s">
-        <v>238</v>
       </c>
       <c r="P4">
         <v>100.01</v>
@@ -7350,7 +7313,7 @@
       </c>
       <c r="T4" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="U4" t="s">
         <v>71</v>
@@ -7380,13 +7343,14 @@
       </c>
       <c r="C5" t="str">
         <f>"o-PK-SUP-POC-230720001-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720001-02</v>
+        <v>o-PK-SUP-POC-230720001-31</v>
       </c>
       <c r="D5" s="30">
         <v>45218</v>
       </c>
-      <c r="E5" t="s">
-        <v>220</v>
+      <c r="E5" t="str">
+        <f>"B-230720001-"&amp;AutoIncrement!A2</f>
+        <v>B-230720001-31</v>
       </c>
       <c r="F5" t="s">
         <v>87</v>
@@ -7401,7 +7365,7 @@
         <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K5" t="s">
         <v>72</v>
@@ -7410,13 +7374,13 @@
         <v>72</v>
       </c>
       <c r="M5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N5" t="s">
+        <v>239</v>
+      </c>
+      <c r="O5" t="s">
         <v>240</v>
-      </c>
-      <c r="O5" t="s">
-        <v>241</v>
       </c>
       <c r="P5">
         <v>100.01</v>
@@ -7429,7 +7393,7 @@
       </c>
       <c r="T5" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="U5" t="s">
         <v>71</v>
@@ -7459,7 +7423,7 @@
       </c>
       <c r="C6" t="str">
         <f>"o-PK-SUP-POC-230720002-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720002-02</v>
+        <v>o-PK-SUP-POC-230720002-31</v>
       </c>
       <c r="D6" s="30">
         <v>45218</v>
@@ -7477,7 +7441,7 @@
         <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K6" t="s">
         <v>72</v>
@@ -7486,13 +7450,13 @@
         <v>72</v>
       </c>
       <c r="M6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N6" t="s">
+        <v>236</v>
+      </c>
+      <c r="O6" t="s">
         <v>237</v>
-      </c>
-      <c r="O6" t="s">
-        <v>238</v>
       </c>
       <c r="P6">
         <v>100.01</v>
@@ -7505,7 +7469,7 @@
       </c>
       <c r="T6" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="U6" t="s">
         <v>71</v>
@@ -7535,7 +7499,7 @@
       </c>
       <c r="C7" t="str">
         <f>"o-PK-SUP-POC-230720002-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720002-02</v>
+        <v>o-PK-SUP-POC-230720002-31</v>
       </c>
       <c r="D7" s="30">
         <v>45218</v>
@@ -7553,7 +7517,7 @@
         <v>69</v>
       </c>
       <c r="J7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K7" t="s">
         <v>72</v>
@@ -7562,13 +7526,13 @@
         <v>72</v>
       </c>
       <c r="M7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N7" t="s">
+        <v>239</v>
+      </c>
+      <c r="O7" t="s">
         <v>240</v>
-      </c>
-      <c r="O7" t="s">
-        <v>241</v>
       </c>
       <c r="P7">
         <v>100.01</v>
@@ -7581,7 +7545,7 @@
       </c>
       <c r="T7" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="U7" t="s">
         <v>71</v>
@@ -7609,7 +7573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F725A8-76DA-4C31-ADD9-93AF9843AA91}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -7624,10 +7588,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B1" t="s">
         <v>332</v>
-      </c>
-      <c r="B1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -7640,7 +7604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6652092F-6BEE-4175-A843-CC7A640F51D9}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -7659,22 +7623,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C1" t="s">
         <v>334</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>335</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>336</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>337</v>
-      </c>
-      <c r="F1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -7702,7 +7666,166 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17D8D98-2282-4C9F-923F-9194E4B05AC4}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="3" max="14" customWidth="true" width="16.21875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="16" max="26" customWidth="true" width="16.21875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="str">
+        <f>"S17_PKSUP-PKCUS"&amp;AutoIncrement!A2</f>
+        <v>S17_PKSUP-PKCUS31</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0</v>
+      </c>
+      <c r="R2" s="5">
+        <v>1</v>
+      </c>
+      <c r="S2" s="5">
+        <v>6</v>
+      </c>
+      <c r="T2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="U2" s="5">
+        <v>31</v>
+      </c>
+      <c r="V2" s="5">
+        <v>12</v>
+      </c>
+      <c r="W2" s="5">
+        <v>2024</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6596C3D8-DABB-4D68-A69F-3FC7822F2C01}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -7739,10 +7862,10 @@
         <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -7839,170 +7962,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17D8D98-2282-4C9F-923F-9194E4B05AC4}">
-  <dimension ref="A1:Y2"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="23.21875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.109375" collapsed="true"/>
-    <col min="3" max="14" customWidth="true" width="16.21875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="41.33203125" collapsed="true"/>
-    <col min="16" max="26" customWidth="true" width="16.21875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>0</v>
-      </c>
-      <c r="R2" s="5">
-        <v>1</v>
-      </c>
-      <c r="S2" s="5">
-        <v>6</v>
-      </c>
-      <c r="T2" s="5">
-        <v>2023</v>
-      </c>
-      <c r="U2" s="5">
-        <v>31</v>
-      </c>
-      <c r="V2" s="5">
-        <v>12</v>
-      </c>
-      <c r="W2" s="5">
-        <v>2024</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433DDF3E-D550-4963-9030-F032BC0321D8}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8012,36 +7977,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="29" t="s">
-        <v>201</v>
-      </c>
       <c r="E1" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="41">
-        <v>45232</v>
+        <v>45244</v>
       </c>
       <c r="B2" s="41">
-        <v>45235</v>
+        <v>45247</v>
       </c>
       <c r="C2" s="41">
-        <v>45245</v>
+        <v>45257</v>
       </c>
       <c r="D2" s="40">
-        <v>45268</v>
+        <v>45301</v>
       </c>
       <c r="E2" s="40">
-        <v>45332</v>
+        <v>45361</v>
       </c>
     </row>
   </sheetData>
@@ -8049,12 +8014,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D46D62-1A05-4CC2-A672-78B90F2AFB42}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8064,13 +8029,13 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
-        <f>"r"&amp;'TC19- Sales Order No'!$A$2&amp;"-04"</f>
-        <v>rss1702-2310001-04</v>
+        <f>"r"&amp;'TC19- Sales Order No'!$A$2&amp;"-03"</f>
+        <v>rss1731-2310001-03</v>
       </c>
     </row>
   </sheetData>
@@ -8078,12 +8043,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632FFAE2-9695-4BBF-A4B6-845817944B45}">
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView topLeftCell="Q2" workbookViewId="0">
-      <selection activeCell="U27" sqref="U26:U27"/>
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8135,31 +8100,31 @@
         <v>151</v>
       </c>
       <c r="N1" t="s">
+        <v>201</v>
+      </c>
+      <c r="O1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" t="s">
         <v>202</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>348</v>
+      </c>
+      <c r="R1" t="s">
         <v>204</v>
       </c>
-      <c r="P1" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>350</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>206</v>
+      </c>
+      <c r="T1" t="s">
+        <v>207</v>
+      </c>
+      <c r="U1" t="s">
         <v>205</v>
       </c>
-      <c r="S1" t="s">
-        <v>207</v>
-      </c>
-      <c r="T1" t="s">
-        <v>208</v>
-      </c>
-      <c r="U1" t="s">
-        <v>206</v>
-      </c>
       <c r="V1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -8393,7 +8358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3919EC5C-738D-46A4-B507-DE2D70B89DAC}">
   <dimension ref="A1:V6"/>
   <sheetViews>
@@ -8447,28 +8412,28 @@
         <v>151</v>
       </c>
       <c r="N1" t="s">
+        <v>201</v>
+      </c>
+      <c r="O1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" t="s">
         <v>202</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>204</v>
       </c>
-      <c r="P1" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>206</v>
+      </c>
+      <c r="S1" t="s">
+        <v>207</v>
+      </c>
+      <c r="T1" t="s">
         <v>205</v>
       </c>
-      <c r="R1" t="s">
-        <v>207</v>
-      </c>
-      <c r="S1" t="s">
-        <v>208</v>
-      </c>
-      <c r="T1" t="s">
-        <v>206</v>
-      </c>
       <c r="U1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -8691,12 +8656,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E777727B-1DDD-4CFF-AA09-5D5BC85D3018}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8721,7 +8686,7 @@
         <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -8797,12 +8762,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58D9144-0E0B-49C9-886E-4A2CDDD2CEB0}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" activeCellId="1" sqref="D8 C8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8812,34 +8777,34 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>200</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="n">
         <f>'TC55- New Outbound Date'!A2</f>
-        <v>45232.0</v>
+        <v>45244.0</v>
       </c>
       <c r="B2" s="41" t="n">
         <f>'TC55- New Outbound Date'!B2</f>
-        <v>45235.0</v>
+        <v>45247.0</v>
       </c>
       <c r="C2" s="41" t="n">
         <f>'TC55- New Outbound Date'!C2</f>
-        <v>45245.0</v>
+        <v>45257.0</v>
       </c>
       <c r="D2" s="40" t="n">
         <f>'TC55- New Outbound Date'!D2</f>
-        <v>45268.0</v>
+        <v>45301.0</v>
       </c>
     </row>
   </sheetData>
@@ -8847,12 +8812,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916ABB38-A115-43EF-A0AC-CEE6A4BC3E6C}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8862,13 +8827,13 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
-        <f>'TC55- Request No'!$A$2</f>
-        <v>rss1702-2310001-04</v>
+        <f>"r"&amp;'TC19- Sales Order No'!$A$2&amp;"-04"</f>
+        <v>rss1731-2310001-04</v>
       </c>
     </row>
   </sheetData>
@@ -8876,19 +8841,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798D413F-7C90-4167-9ECC-358646B148B3}">
   <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" customWidth="true" width="14.6640625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="26.33203125" collapsed="true"/>
-    <col min="4" max="6" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="24.88671875" collapsed="true"/>
     <col min="8" max="32" customWidth="true" width="14.6640625" collapsed="true"/>
     <col min="33" max="33" customWidth="true" width="18.0" collapsed="true"/>
@@ -8899,124 +8865,124 @@
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" t="s">
         <v>255</v>
       </c>
-      <c r="B1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>218</v>
       </c>
-      <c r="E1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F1" t="s">
-        <v>219</v>
-      </c>
       <c r="G1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H1" t="s">
         <v>221</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>222</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>223</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>224</v>
-      </c>
-      <c r="K1" t="s">
-        <v>225</v>
       </c>
       <c r="L1" t="s">
         <v>128</v>
       </c>
       <c r="M1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N1" t="s">
+        <v>256</v>
+      </c>
+      <c r="O1" t="s">
         <v>257</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q1" t="s">
         <v>258</v>
       </c>
-      <c r="P1" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>259</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>260</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
+        <v>264</v>
+      </c>
+      <c r="U1" t="s">
+        <v>267</v>
+      </c>
+      <c r="V1" t="s">
+        <v>268</v>
+      </c>
+      <c r="W1" t="s">
+        <v>231</v>
+      </c>
+      <c r="X1" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>270</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC1" t="s">
         <v>261</v>
       </c>
-      <c r="T1" t="s">
-        <v>265</v>
-      </c>
-      <c r="U1" t="s">
-        <v>268</v>
-      </c>
-      <c r="V1" t="s">
-        <v>269</v>
-      </c>
-      <c r="W1" t="s">
-        <v>232</v>
-      </c>
-      <c r="X1" t="s">
-        <v>233</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="AD1" t="s">
         <v>266</v>
       </c>
-      <c r="Z1" t="s">
-        <v>270</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>271</v>
       </c>
-      <c r="AB1" t="s">
-        <v>236</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AL1" t="s">
         <v>262</v>
       </c>
-      <c r="AD1" t="s">
-        <v>267</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>272</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>273</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>243</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>244</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>245</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>246</v>
-      </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>247</v>
       </c>
-      <c r="AL1" t="s">
-        <v>263</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>248</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.3">
@@ -9028,13 +8994,14 @@
       </c>
       <c r="C2" t="str">
         <f>"o-PK-SUP-POC-230720003-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720003-02</v>
+        <v>o-PK-SUP-POC-230720003-31</v>
       </c>
       <c r="D2" s="30">
         <v>45218</v>
       </c>
-      <c r="F2" t="s">
-        <v>220</v>
+      <c r="F2" t="str">
+        <f>"B-230720001-"&amp;AutoIncrement!A2</f>
+        <v>B-230720001-31</v>
       </c>
       <c r="G2" t="s">
         <v>87</v>
@@ -9049,7 +9016,7 @@
         <v>69</v>
       </c>
       <c r="K2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L2" t="s">
         <v>72</v>
@@ -9058,13 +9025,13 @@
         <v>72</v>
       </c>
       <c r="P2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="W2" t="s">
+        <v>239</v>
+      </c>
+      <c r="X2" t="s">
         <v>240</v>
-      </c>
-      <c r="X2" t="s">
-        <v>241</v>
       </c>
       <c r="Y2">
         <v>100.01</v>
@@ -9077,7 +9044,7 @@
       </c>
       <c r="AG2" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1702-2310001</v>
+        <v>ss1731-2310001</v>
       </c>
       <c r="AH2" t="s">
         <v>71</v>
@@ -9104,7 +9071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A92A14-B736-4BE2-B5C8-4BD774DAC054}">
   <dimension ref="A1:W4"/>
   <sheetViews>
@@ -9122,328 +9089,278 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>275</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>165</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="44" t="s">
         <v>283</v>
       </c>
-      <c r="O1" s="44" t="s">
+      <c r="P1" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>303</v>
-      </c>
       <c r="G2" s="45" t="s">
+        <v>291</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>294</v>
-      </c>
       <c r="J2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>303</v>
-      </c>
       <c r="G3" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>294</v>
-      </c>
       <c r="J3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>303</v>
-      </c>
       <c r="G4" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>294</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3527525D-DCF3-42E0-8A83-320500061703}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" customWidth="true" width="20.77734375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>220</v>
-      </c>
-      <c r="B4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -9453,7 +9370,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9516,7 +9433,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E2" s="13">
         <v>0.5</v>
@@ -9552,7 +9469,7 @@
       </c>
       <c r="D3" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E3" s="13">
         <v>0.5</v>
@@ -9588,7 +9505,7 @@
       </c>
       <c r="D4" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E4" s="13">
         <v>0.5</v>
@@ -9624,7 +9541,7 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E5" s="13">
         <v>0.5</v>
@@ -9660,7 +9577,7 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="E6" s="14">
         <v>0.5</v>
@@ -9691,6 +9608,56 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3527525D-DCF3-42E0-8A83-320500061703}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" customWidth="true" width="20.77734375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07131E43-540D-4AB5-B799-C1C9E8C3480D}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -9706,15 +9673,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" t="s">
         <v>321</v>
-      </c>
-      <c r="B1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B2" s="40">
         <v>45125</v>
@@ -9722,7 +9689,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B3" s="40">
         <v>45125</v>
@@ -9730,7 +9697,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B4" s="40">
         <v>45125</v>
@@ -9738,7 +9705,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B5" s="40">
         <v>45125</v>
@@ -9746,7 +9713,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B6" s="40">
         <v>45125</v>
@@ -9754,7 +9721,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B7" s="40">
         <v>45125</v>
@@ -9762,7 +9729,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B8" s="40">
         <v>45125</v>
@@ -9773,12 +9740,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D61966F-68FA-4203-8F7A-1605789961DD}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9789,37 +9756,37 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>324</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>'TC51- Outbound Details'!$C$2</f>
-        <v>o-PK-SUP-POC-230720001-02</v>
+        <v>o-PK-SUP-POC-230720001-31</v>
       </c>
       <c r="B2" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>'TC51- Outbound Details'!$C$6</f>
-        <v>o-PK-SUP-POC-230720002-02</v>
+        <v>o-PK-SUP-POC-230720002-31</v>
       </c>
       <c r="B3" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>'TC69- Outbound Details'!$C$2</f>
-        <v>o-PK-SUP-POC-230720003-02</v>
+        <v>o-PK-SUP-POC-230720003-31</v>
       </c>
       <c r="B4" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -9827,7 +9794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256B465A-06B6-4028-A3DE-171E9F4E873E}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -9843,10 +9810,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -9862,7 +9829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813C15B5-BFA5-453B-8BB1-2BD28A10985D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -9879,22 +9846,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C1" t="s">
         <v>334</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>335</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>336</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>337</v>
-      </c>
-      <c r="F1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -9922,12 +9889,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40266E76-E31A-42AB-9082-4A7187A8DFDB}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9942,10 +9909,10 @@
         <v>99</v>
       </c>
       <c r="B1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1" s="50" t="s">
         <v>325</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -9954,10 +9921,10 @@
       </c>
       <c r="B2" t="str">
         <f>'TC75- Outbound Nos'!$B$2</f>
-        <v>o-PK-SUP-POC-231024001</v>
+        <v>o-PK-SUP-POC-231030001</v>
       </c>
       <c r="C2" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -9966,10 +9933,10 @@
       </c>
       <c r="B3" t="str">
         <f>'TC75- Outbound Nos'!$B$3</f>
-        <v>o-PK-SUP-POC-231024002</v>
+        <v>o-PK-SUP-POC-231030002</v>
       </c>
       <c r="C3" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -9978,10 +9945,10 @@
       </c>
       <c r="B4" t="str">
         <f>'TC75- Outbound Nos'!$B$4</f>
-        <v>o-PK-SUP-POC-231024003</v>
+        <v>o-PK-SUP-POC-231031001</v>
       </c>
       <c r="C4" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -9995,8 +9962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66A75C4-CFB3-461E-9746-0710E05709C6}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10067,7 +10034,7 @@
         <v>118</v>
       </c>
       <c r="R1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="S1" t="s">
         <v>119</v>
@@ -10088,7 +10055,7 @@
       </c>
       <c r="B2" s="6" t="str">
         <f>"PKSUPTOPKCUS17001-"&amp;'TC2- ReceivedRequestAddNewPart'!K2&amp;"-0"&amp;AutoIncrement!A2</f>
-        <v>PKSUPTOPKCUS17001-s1702-002</v>
+        <v>PKSUPTOPKCUS17001-s1731-031</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>72</v>
@@ -10116,10 +10083,10 @@
       </c>
       <c r="K2" s="18" t="str">
         <f>"s17"&amp;AutoIncrement!A2</f>
-        <v>s1702</v>
+        <v>s1731</v>
       </c>
       <c r="L2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M2" t="s">
         <v>81</v>
@@ -10132,10 +10099,10 @@
       </c>
       <c r="R2" t="str">
         <f>'TC1-Description'!$A$2</f>
-        <v>s1702</v>
+        <v>s1731</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="T2" t="s">
         <v>101</v>
@@ -10154,7 +10121,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10174,10 +10141,10 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$K$2</f>
-        <v>s1702</v>
+        <v>s1731</v>
       </c>
       <c r="B2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -10218,7 +10185,7 @@
         <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -10230,34 +10197,34 @@
         <v>93</v>
       </c>
       <c r="H1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I1" t="s">
         <v>305</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>306</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>307</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>308</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>309</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>310</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>311</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>312</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>313</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>314</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
@@ -10266,7 +10233,7 @@
         <v>20</v>
       </c>
       <c r="T1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U1" t="s">
         <v>95</v>
@@ -10278,13 +10245,13 @@
         <v>21</v>
       </c>
       <c r="X1" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y1" t="s">
         <v>316</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>317</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>318</v>
       </c>
       <c r="AA1" t="s">
         <v>22</v>
@@ -10293,7 +10260,7 @@
         <v>23</v>
       </c>
       <c r="AC1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
@@ -10326,7 +10293,7 @@
       </c>
       <c r="J2" s="49" t="str">
         <f ca="1">TEXT(TODAY(), "mmm d, yyyy")</f>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R2">
         <v>10</v>
@@ -10395,7 +10362,7 @@
       </c>
       <c r="J3" s="49" t="str">
         <f ca="1" ref="J3:J6" si="0" t="shared">TEXT(TODAY(), "mmm d, yyyy")</f>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R3">
         <v>10</v>
@@ -10464,7 +10431,7 @@
       </c>
       <c r="J4" s="49" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R4">
         <v>10</v>
@@ -10533,7 +10500,7 @@
       </c>
       <c r="J5" s="49" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R5">
         <v>10</v>
@@ -10589,7 +10556,7 @@
         <v>89</v>
       </c>
       <c r="F6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G6" s="46">
         <v>0.5</v>
@@ -10602,7 +10569,7 @@
       </c>
       <c r="J6" s="49" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>Oct 25, 2023</v>
+        <v>Oct 31, 2023</v>
       </c>
       <c r="R6">
         <v>10</v>

</xml_diff>

<commit_message>
Fix test objects S17
</commit_message>
<xml_diff>
--- a/Excel Files/Scenario 17/S17_TestCases_Data.xlsx
+++ b/Excel Files/Scenario 17/S17_TestCases_Data.xlsx
@@ -1,83 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasin\git\tb-ttap-brivge-v2\Excel Files\Scenario 17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E6E612-A2B0-4DED-A17E-D71FBE28C544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{F1C05B8F-9149-4E9E-92EC-38E5ECD39899}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="567" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="59" firstSheet="56" tabRatio="567" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="AutoIncrement" sheetId="86" r:id="rId1"/>
-    <sheet name="TC1- Add New Parts" sheetId="2" r:id="rId2"/>
-    <sheet name="TC1-Description" sheetId="87" r:id="rId3"/>
-    <sheet name="TC1.1- Payment Terms" sheetId="1" r:id="rId4"/>
-    <sheet name="TC1.2- Shipping Route" sheetId="3" r:id="rId5"/>
-    <sheet name="TC2- Contract Parts Info" sheetId="5" r:id="rId6"/>
-    <sheet name="TC2- ReceivedRequestAddNewPart" sheetId="6" r:id="rId7"/>
-    <sheet name="TC3-Description" sheetId="74" r:id="rId8"/>
-    <sheet name="TC5- Contract Parts" sheetId="65" r:id="rId9"/>
-    <sheet name="TC6- Part List " sheetId="7" r:id="rId10"/>
-    <sheet name="TC6- Contract Route Code" sheetId="75" r:id="rId11"/>
-    <sheet name="TC7- Request to Parts Master" sheetId="8" r:id="rId12"/>
-    <sheet name="TC7- RequestNo" sheetId="76" r:id="rId13"/>
-    <sheet name="TC8- Contract Parts Info" sheetId="16" r:id="rId14"/>
-    <sheet name="TC9- Contract List" sheetId="17" r:id="rId15"/>
-    <sheet name="TC10- Parts List" sheetId="55" r:id="rId16"/>
-    <sheet name="T11- RequestNo" sheetId="77" r:id="rId17"/>
-    <sheet name="TC16- Tenth Day Period" sheetId="96" r:id="rId18"/>
-    <sheet name="TC16- New Firm Qty" sheetId="18" r:id="rId19"/>
-    <sheet name="TC16- New Inbound Date1" sheetId="35" r:id="rId20"/>
-    <sheet name="TC17- Regular Customer No" sheetId="79" r:id="rId21"/>
-    <sheet name="TC19-Delivery Plan" sheetId="37" r:id="rId22"/>
-    <sheet name="TC19- Order Price" sheetId="36" r:id="rId23"/>
-    <sheet name="TC19- Sales Order No" sheetId="80" r:id="rId24"/>
-    <sheet name="TC21- Forecast Change" sheetId="34" r:id="rId25"/>
-    <sheet name="TC21- RequestNo" sheetId="56" r:id="rId26"/>
-    <sheet name="TC22- Parts Detail" sheetId="38" r:id="rId27"/>
-    <sheet name="TC26- Parts Detail" sheetId="57" r:id="rId28"/>
-    <sheet name="TC27-Change Firm Qty" sheetId="21" r:id="rId29"/>
-    <sheet name=" T27- Change Inbound Date" sheetId="23" r:id="rId30"/>
-    <sheet name="TC27- Request No" sheetId="88" r:id="rId31"/>
-    <sheet name="TC28- Parts Detail" sheetId="89" r:id="rId32"/>
-    <sheet name="T31-Parts Detail" sheetId="90" r:id="rId33"/>
-    <sheet name="TC32- Sales Order Info" sheetId="25" r:id="rId34"/>
-    <sheet name="TC33- Customer Forecast Detail" sheetId="26" r:id="rId35"/>
-    <sheet name="TC34- Request No" sheetId="91" r:id="rId36"/>
-    <sheet name="T35- Parts Detail" sheetId="28" r:id="rId37"/>
-    <sheet name="TC38- Change Firm Qty" sheetId="31" r:id="rId38"/>
-    <sheet name="TC40- Units Part Master" sheetId="33" r:id="rId39"/>
-    <sheet name="TC41- Temp Firm Quantity" sheetId="41" r:id="rId40"/>
-    <sheet name="TC41.1-Temp Outbound Date" sheetId="42" r:id="rId41"/>
-    <sheet name="TC42- Edit Firm Quantity1" sheetId="45" r:id="rId42"/>
-    <sheet name="TC42- Request No" sheetId="92" r:id="rId43"/>
-    <sheet name="TC43- Parts Detail" sheetId="47" r:id="rId44"/>
-    <sheet name="TC46- Parts Detail" sheetId="48" r:id="rId45"/>
-    <sheet name="TC50- Request No" sheetId="93" r:id="rId46"/>
-    <sheet name="TC51- Outbound Details" sheetId="49" r:id="rId47"/>
-    <sheet name="TC54-Purchase Amount By Sup" sheetId="81" r:id="rId48"/>
-    <sheet name="TC55- Complete Deliveries List" sheetId="82" r:id="rId49"/>
-    <sheet name="TC55- New Firm Quantity" sheetId="52" r:id="rId50"/>
-    <sheet name="TC55- New Outbound Date" sheetId="53" r:id="rId51"/>
-    <sheet name="TC55- Request No" sheetId="94" r:id="rId52"/>
-    <sheet name="TC56- Part Details" sheetId="54" r:id="rId53"/>
-    <sheet name="TC60- Parts Detail1" sheetId="59" r:id="rId54"/>
-    <sheet name="TC63- New Firm Quantity" sheetId="60" r:id="rId55"/>
-    <sheet name="TC63- New Oubound Date" sheetId="61" r:id="rId56"/>
-    <sheet name="TC63- Request No" sheetId="95" r:id="rId57"/>
-    <sheet name="TC69- Outbound Details" sheetId="62" r:id="rId58"/>
-    <sheet name="TC71 &amp; 72- CargoTrackingDetail " sheetId="63" r:id="rId59"/>
-    <sheet name="T73- Shipping Detail" sheetId="67" r:id="rId60"/>
-    <sheet name="TC75- Customer Inbound Details" sheetId="69" r:id="rId61"/>
-    <sheet name="TC75- Outbound Nos" sheetId="71" r:id="rId62"/>
-    <sheet name="TC76- Purchase Amount By Sup" sheetId="84" r:id="rId63"/>
-    <sheet name="TC76- Complete Deliveries List" sheetId="85" r:id="rId64"/>
-    <sheet name="TC78 - Supplier SellerGIInvoice" sheetId="72" r:id="rId65"/>
+    <sheet name="AutoIncrement" r:id="rId1" sheetId="86"/>
+    <sheet name="TC1- Add New Parts" r:id="rId2" sheetId="2"/>
+    <sheet name="TC1-Description" r:id="rId3" sheetId="87"/>
+    <sheet name="TC1.1- Payment Terms" r:id="rId4" sheetId="1"/>
+    <sheet name="TC1.2- Shipping Route" r:id="rId5" sheetId="3"/>
+    <sheet name="TC2- Contract Parts Info" r:id="rId6" sheetId="5"/>
+    <sheet name="TC2- ReceivedRequestAddNewPart" r:id="rId7" sheetId="6"/>
+    <sheet name="TC3-Description" r:id="rId8" sheetId="74"/>
+    <sheet name="TC5- Contract Parts" r:id="rId9" sheetId="65"/>
+    <sheet name="TC6- Part List " r:id="rId10" sheetId="7"/>
+    <sheet name="TC6- Contract Route Code" r:id="rId11" sheetId="75"/>
+    <sheet name="TC7- Request to Parts Master" r:id="rId12" sheetId="8"/>
+    <sheet name="TC7- RequestNo" r:id="rId13" sheetId="76"/>
+    <sheet name="TC8- Contract Parts Info" r:id="rId14" sheetId="16"/>
+    <sheet name="TC9- Contract List" r:id="rId15" sheetId="17"/>
+    <sheet name="TC10- Parts List" r:id="rId16" sheetId="55"/>
+    <sheet name="T11- RequestNo" r:id="rId17" sheetId="77"/>
+    <sheet name="TC16- Tenth Day Period" r:id="rId18" sheetId="96"/>
+    <sheet name="TC16- New Firm Qty" r:id="rId19" sheetId="18"/>
+    <sheet name="TC16- New Inbound Date1" r:id="rId20" sheetId="35"/>
+    <sheet name="TC17- Regular Customer No" r:id="rId21" sheetId="79"/>
+    <sheet name="TC19-Delivery Plan" r:id="rId22" sheetId="37"/>
+    <sheet name="TC19- Order Price" r:id="rId23" sheetId="36"/>
+    <sheet name="TC19- Sales Order No" r:id="rId24" sheetId="80"/>
+    <sheet name="TC21- Forecast Change" r:id="rId25" sheetId="34"/>
+    <sheet name="TC21- RequestNo" r:id="rId26" sheetId="56"/>
+    <sheet name="TC22- Parts Detail" r:id="rId27" sheetId="38"/>
+    <sheet name="TC26- Parts Detail" r:id="rId28" sheetId="57"/>
+    <sheet name="TC27-Change Firm Qty" r:id="rId29" sheetId="21"/>
+    <sheet name=" T27- Change Inbound Date" r:id="rId30" sheetId="23"/>
+    <sheet name="TC27- Request No" r:id="rId31" sheetId="88"/>
+    <sheet name="TC28- Parts Detail" r:id="rId32" sheetId="89"/>
+    <sheet name="T31-Parts Detail" r:id="rId33" sheetId="90"/>
+    <sheet name="TC32- Sales Order Info" r:id="rId34" sheetId="25"/>
+    <sheet name="TC33- Customer Forecast Detail" r:id="rId35" sheetId="26"/>
+    <sheet name="TC34- Request No" r:id="rId36" sheetId="91"/>
+    <sheet name="T35- Parts Detail" r:id="rId37" sheetId="28"/>
+    <sheet name="TC38- Change Firm Qty" r:id="rId38" sheetId="31"/>
+    <sheet name="TC40- Units Part Master" r:id="rId39" sheetId="33"/>
+    <sheet name="TC41- Temp Firm Quantity" r:id="rId40" sheetId="41"/>
+    <sheet name="TC41.1-Temp Outbound Date" r:id="rId41" sheetId="42"/>
+    <sheet name="TC42- Edit Firm Quantity1" r:id="rId42" sheetId="45"/>
+    <sheet name="TC42- Request No" r:id="rId43" sheetId="92"/>
+    <sheet name="TC43- Parts Detail" r:id="rId44" sheetId="47"/>
+    <sheet name="TC46- Parts Detail" r:id="rId45" sheetId="48"/>
+    <sheet name="TC50- Request No" r:id="rId46" sheetId="93"/>
+    <sheet name="TC51- Outbound Details" r:id="rId47" sheetId="49"/>
+    <sheet name="TC54-Purchase Amount By Sup" r:id="rId48" sheetId="81"/>
+    <sheet name="TC55- Complete Deliveries List" r:id="rId49" sheetId="82"/>
+    <sheet name="TC55- New Firm Quantity" r:id="rId50" sheetId="52"/>
+    <sheet name="TC55- New Outbound Date" r:id="rId51" sheetId="53"/>
+    <sheet name="TC55- Request No" r:id="rId52" sheetId="94"/>
+    <sheet name="TC56- Part Details" r:id="rId53" sheetId="54"/>
+    <sheet name="TC60- Parts Detail1" r:id="rId54" sheetId="59"/>
+    <sheet name="TC63- New Firm Quantity" r:id="rId55" sheetId="60"/>
+    <sheet name="TC63- New Oubound Date" r:id="rId56" sheetId="61"/>
+    <sheet name="TC63- Request No" r:id="rId57" sheetId="95"/>
+    <sheet name="TC69- Outbound Details" r:id="rId58" sheetId="62"/>
+    <sheet name="TC71 &amp; 72- CargoTrackingDetail " r:id="rId59" sheetId="63"/>
+    <sheet name="T73- Shipping Detail" r:id="rId60" sheetId="67"/>
+    <sheet name="TC75- Customer Inbound Details" r:id="rId61" sheetId="69"/>
+    <sheet name="TC75- Outbound Nos" r:id="rId62" sheetId="71"/>
+    <sheet name="TC76- Purchase Amount By Sup" r:id="rId63" sheetId="84"/>
+    <sheet name="TC76- Complete Deliveries List" r:id="rId64" sheetId="85"/>
+    <sheet name="TC78 - Supplier SellerGIInvoice" r:id="rId65" sheetId="72"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId66"/>
@@ -87,7 +87,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="369">
   <si>
     <t>NEW/MOD</t>
   </si>
@@ -1153,30 +1153,6 @@
     <t>Auto Generate Tenth Day Period</t>
   </si>
   <si>
-    <t>R-PK-CUS-POC-2310210</t>
-  </si>
-  <si>
-    <t>R-PK-CUS-POC-2310211</t>
-  </si>
-  <si>
-    <t>cs1731-2310001</t>
-  </si>
-  <si>
-    <t>ss1731-2310001</t>
-  </si>
-  <si>
-    <t>R-PK-CUS-POC-2310212</t>
-  </si>
-  <si>
-    <t>o-PK-SUP-POC-231030001</t>
-  </si>
-  <si>
-    <t>o-PK-SUP-POC-231030002</t>
-  </si>
-  <si>
-    <t>o-PK-SUP-POC-231031001</t>
-  </si>
-  <si>
     <t>PKS2310071</t>
   </si>
   <si>
@@ -1186,13 +1162,46 @@
     <t>PKS2310073</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>R-PK-CUS-POC-2311007</t>
-  </si>
-  <si>
-    <t>CR-PK-CUS-POC-2311003</t>
+    <t>35</t>
+  </si>
+  <si>
+    <t>R-PK-CUS-POC-2311012</t>
+  </si>
+  <si>
+    <t>CR-PK-CUS-POC-2311006</t>
+  </si>
+  <si>
+    <t>R-PK-CUS-POC-2311013</t>
+  </si>
+  <si>
+    <t>R-PK-CUS-POC-2311014</t>
+  </si>
+  <si>
+    <t>cs1735-2311001</t>
+  </si>
+  <si>
+    <t>ss1735-2311001</t>
+  </si>
+  <si>
+    <t>R-PK-CUS-POC-2311015</t>
+  </si>
+  <si>
+    <t>o-PK-SUP-POC-231106001</t>
+  </si>
+  <si>
+    <t>o-PK-SUP-POC-231106002</t>
+  </si>
+  <si>
+    <t>o-PK-SUP-POC-231106003</t>
+  </si>
+  <si>
+    <t>PKS2311001</t>
+  </si>
+  <si>
+    <t>PKS2311002</t>
+  </si>
+  <si>
+    <t>PKS2311003</t>
   </si>
 </sst>
 </file>
@@ -1391,133 +1400,133 @@
     </border>
   </borders>
   <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="9"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="43"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="58">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="1" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="3" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="15" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="2"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="2"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="2"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="37" xfId="2"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="15" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="9" xfId="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="9" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="10" numFmtId="15" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 4" xfId="4" xr:uid="{6AC67C4D-7067-4C0A-A103-9600AB310598}"/>
     <cellStyle name="Normal 6 2" xfId="3" xr:uid="{C192ED1A-D084-4E48-A012-E104EE76E27F}"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1724,7 +1733,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData refreshError="1" sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1735,10 +1744,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1773,7 +1782,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1808,7 +1817,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1902,21 +1911,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1933,7 +1942,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1985,24 +1994,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CEAEA8-8A66-492C-8B01-278DD5AD4FC8}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CEAEA8-8A66-492C-8B01-278DD5AD4FC8}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -2017,7 +2026,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="54" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
@@ -2027,13 +2036,13 @@
       <c r="D3" s="52"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605C6405-307C-4F3C-9FCD-55F683B2D544}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605C6405-307C-4F3C-9FCD-55F683B2D544}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
@@ -2041,13 +2050,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="44.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="44.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2085,7 +2094,7 @@
       </c>
       <c r="D2" t="str">
         <f>'TC2- Contract Parts Info'!D2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E2" t="s">
         <v>100</v>
@@ -2109,7 +2118,7 @@
       </c>
       <c r="D3" t="str">
         <f>'TC2- Contract Parts Info'!D3</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E3" t="s">
         <v>100</v>
@@ -2133,7 +2142,7 @@
       </c>
       <c r="D4" t="str">
         <f>'TC2- Contract Parts Info'!D4</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E4" t="s">
         <v>100</v>
@@ -2157,7 +2166,7 @@
       </c>
       <c r="D5" t="str">
         <f>'TC2- Contract Parts Info'!D5</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E5" t="s">
         <v>100</v>
@@ -2171,12 +2180,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0F2314-8449-48D7-9DA6-41BD97221C6F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0F2314-8449-48D7-9DA6-41BD97221C6F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2185,8 +2194,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -2196,17 +2205,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8051FE61-E748-44E4-BEB7-407CF6D42E4B}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8051FE61-E748-44E4-BEB7-407CF6D42E4B}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -2214,10 +2223,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="16" width="24.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="4" max="16" customWidth="true" width="24.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -2315,13 +2324,13 @@
       <c r="P2" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8B231-F5F1-4BD6-B711-847644B80026}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8B231-F5F1-4BD6-B711-847644B80026}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
@@ -2329,7 +2338,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -2339,17 +2348,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79AEE038-38D4-4203-93E5-BE48DBE5A31B}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79AEE038-38D4-4203-93E5-BE48DBE5A31B}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
@@ -2357,7 +2366,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2383,7 +2392,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="B2" s="25">
         <v>1</v>
@@ -2402,13 +2411,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E58BD6D-388E-469A-82FD-BA926414BBAA}">
-  <dimension ref="A1:AC6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E58BD6D-388E-469A-82FD-BA926414BBAA}">
+  <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -2416,13 +2425,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="31.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="8" width="31.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="12" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="13" max="17" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="20" max="22" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="31.5546875" collapsed="true"/>
+    <col min="4" max="8" customWidth="true" width="31.88671875" collapsed="true"/>
+    <col min="9" max="12" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="13" max="17" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="20" max="22" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="25.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
@@ -2544,7 +2553,7 @@
       </c>
       <c r="J2" t="str">
         <f ca="1">TEXT(TODAY(), "mmm d, yyyy")</f>
-        <v>Nov 5, 2023</v>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R2">
         <v>10</v>
@@ -2612,8 +2621,8 @@
         <v>8</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J6" ca="1" si="0">TEXT(TODAY(), "mmm d, yyyy")</f>
-        <v>Nov 5, 2023</v>
+        <f ca="1" ref="J3:J6" si="0" t="shared">TEXT(TODAY(), "mmm d, yyyy")</f>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R3">
         <v>10</v>
@@ -2681,8 +2690,8 @@
         <v>10</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Nov 5, 2023</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R4">
         <v>10</v>
@@ -2750,8 +2759,8 @@
         <v>10</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Nov 5, 2023</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R5">
         <v>10</v>
@@ -2819,8 +2828,8 @@
         <v>101</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Nov 5, 2023</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R6">
         <v>10</v>
@@ -2861,14 +2870,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A0B8AB-F755-4013-A062-674BB4F9EE7C}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A0B8AB-F755-4013-A062-674BB4F9EE7C}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -2876,9 +2885,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="33.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="7" width="33.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="3" customWidth="true" width="33.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="44.33203125" collapsed="true"/>
+    <col min="5" max="7" customWidth="true" width="33.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -2916,7 +2925,7 @@
       </c>
       <c r="D2" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E2" t="s">
         <v>100</v>
@@ -2940,7 +2949,7 @@
       </c>
       <c r="D3" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E3" t="s">
         <v>100</v>
@@ -2964,7 +2973,7 @@
       </c>
       <c r="D4" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E4" t="s">
         <v>100</v>
@@ -2988,7 +2997,7 @@
       </c>
       <c r="D5" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E5" t="s">
         <v>100</v>
@@ -3012,7 +3021,7 @@
       </c>
       <c r="D6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E6" t="s">
         <v>100</v>
@@ -3026,13 +3035,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01215CAA-E5A5-4F8D-B96F-587BD8F24CF3}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01215CAA-E5A5-4F8D-B96F-587BD8F24CF3}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -3040,8 +3049,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -3055,49 +3064,49 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$K$2</f>
-        <v>s1733</v>
+        <v>s1735</v>
       </c>
       <c r="B2" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F8C9AC-BFC1-4F74-A888-81960B4CD9E6}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F8C9AC-BFC1-4F74-A888-81960B4CD9E6}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+    <row ht="15" r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.35">
+    <row ht="15" r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="56" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), 10, 22)+((INT((TODAY()-DATE(YEAR(TODAY()),10,21))/10))*10),"mmm d, yyyy") &amp; " ~ " &amp; TEXT(DATE(YEAR(TODAY()), 10, 31)+((INT((TODAY()-DATE(YEAR(TODAY()),10,21))/10))*10),"mmm d, yyyy")</f>
         <v>Nov 1, 2023 ~ Nov 10, 2023</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EB5BCC-E864-435B-857D-D35862E35EB0}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EB5BCC-E864-435B-857D-D35862E35EB0}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
@@ -3105,14 +3114,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="14.4" r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -3207,13 +3216,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307750ED-3D08-4077-9AE4-0CE85FD915D6}">
-  <dimension ref="A1:P6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307750ED-3D08-4077-9AE4-0CE85FD915D6}">
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
@@ -3221,13 +3230,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="48.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="8" width="28.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="44" customWidth="1" collapsed="1"/>
-    <col min="10" max="16" width="28.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="48.88671875" collapsed="true"/>
+    <col min="5" max="8" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="44.0" collapsed="true"/>
+    <col min="10" max="16" customWidth="true" width="28.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -3496,21 +3505,21 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A15540F-447C-472A-9FC9-ECC8F627E6F5}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A15540F-447C-472A-9FC9-ECC8F627E6F5}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J13" sqref="J13:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="35.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="35.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -3530,13 +3539,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEDC36B2-2345-4809-9DF4-82A2306D2076}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEDC36B2-2345-4809-9DF4-82A2306D2076}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3544,9 +3553,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="7.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -3556,17 +3565,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01064E38-B985-4C88-953C-91312F7E645E}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01064E38-B985-4C88-953C-91312F7E645E}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
@@ -3617,14 +3626,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688A99D8-A546-4793-BF80-17BCE9AC2E6A}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688A99D8-A546-4793-BF80-17BCE9AC2E6A}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -3632,7 +3641,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="24.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -3684,12 +3693,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F8BF62-0F7A-4A26-AEBF-44DCC1217B1A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F8BF62-0F7A-4A26-AEBF-44DCC1217B1A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3698,8 +3707,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -3709,26 +3718,26 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E387D73C-C5A5-49CC-84DA-30FD52F9787C}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E387D73C-C5A5-49CC-84DA-30FD52F9787C}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -3798,12 +3807,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C93116F-C081-465D-B251-5D5DDE8C10B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C93116F-C081-465D-B251-5D5DDE8C10B4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3812,8 +3821,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -3824,31 +3833,31 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>"r"&amp;'TC17- Regular Customer No'!$A$2&amp;"-"&amp;"01"</f>
-        <v>rcs1731-2310001-01</v>
+        <v>rcs1735-2311001-01</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8295D9FD-18AA-4414-88C1-5A2C28BBBFD0}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8295D9FD-18AA-4414-88C1-5A2C28BBBFD0}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="17.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.88671875" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -3961,23 +3970,23 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA8620A-4A8E-4AAE-B2CE-F0EEF0338C09}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA8620A-4A8E-4AAE-B2CE-F0EEF0338C09}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="12" width="27.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="3" max="12" customWidth="true" width="27.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -4089,13 +4098,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAA4611-B951-475F-8E0F-A612CCEB920F}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAA4611-B951-475F-8E0F-A612CCEB920F}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A6"/>
@@ -4103,10 +4112,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="10" width="20" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="36.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.77734375" collapsed="true"/>
+    <col min="5" max="10" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -4214,13 +4223,13 @@
       <c r="F6" s="31"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2023D2A2-A733-426A-8565-677FAAC3BE3A}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2023D2A2-A733-426A-8565-677FAAC3BE3A}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
@@ -4228,7 +4237,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -4239,17 +4248,17 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$K$2</f>
-        <v>s1733</v>
+        <v>s1735</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398FF2F2-BB87-4EBD-BB67-BC80830F281F}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398FF2F2-BB87-4EBD-BB67-BC80830F281F}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -4257,7 +4266,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="24.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="7" customWidth="true" width="24.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -4283,13 +4292,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E643A149-B87E-4DD7-A3D9-F8B3E4DB4447}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E643A149-B87E-4DD7-A3D9-F8B3E4DB4447}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
@@ -4297,7 +4306,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -4308,17 +4317,17 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>"r"&amp;'TC17- Regular Customer No'!$A$2&amp;"-"&amp;"02"</f>
-        <v>rcs1731-2310001-02</v>
+        <v>rcs1735-2311001-02</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43AE63B-7AAE-42E4-89C6-4F58557162BE}">
-  <dimension ref="A1:Q3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43AE63B-7AAE-42E4-89C6-4F58557162BE}">
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
@@ -4326,19 +4335,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.21875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="15.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -4481,12 +4490,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BE52D5-E46D-41A4-A6A6-4DDA1680687F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BE52D5-E46D-41A4-A6A6-4DDA1680687F}">
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -4495,11 +4504,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="20.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="25.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="19" width="20.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="20.21875" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="25.21875" collapsed="true"/>
+    <col min="7" max="19" customWidth="true" width="20.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -4639,13 +4648,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA77A46-DDE3-43E3-B541-11491347B436}">
-  <dimension ref="A1:AE6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA77A46-DDE3-43E3-B541-11491347B436}">
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
@@ -4653,14 +4662,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="16" width="17" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="18" max="31" width="28.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="6" max="16" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="18" max="31" customWidth="true" width="28.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
@@ -4755,7 +4764,7 @@
       </c>
       <c r="D2" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1731-2310001</v>
+        <v>cs1735-2311001</v>
       </c>
       <c r="E2" t="s">
         <v>72</v>
@@ -4836,7 +4845,7 @@
       </c>
       <c r="D3" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1731-2310001</v>
+        <v>cs1735-2311001</v>
       </c>
       <c r="E3" t="s">
         <v>72</v>
@@ -4917,7 +4926,7 @@
       </c>
       <c r="D4" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1731-2310001</v>
+        <v>cs1735-2311001</v>
       </c>
       <c r="E4" t="s">
         <v>72</v>
@@ -4998,7 +5007,7 @@
       </c>
       <c r="D5" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1731-2310001</v>
+        <v>cs1735-2311001</v>
       </c>
       <c r="E5" t="s">
         <v>72</v>
@@ -5079,7 +5088,7 @@
       </c>
       <c r="D6" t="str">
         <f>'TC17- Regular Customer No'!$A$2</f>
-        <v>cs1731-2310001</v>
+        <v>cs1735-2311001</v>
       </c>
       <c r="E6" t="s">
         <v>72</v>
@@ -5150,13 +5159,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C097B8-9E0B-4919-8936-C8FA44A90F17}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C097B8-9E0B-4919-8936-C8FA44A90F17}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D19" sqref="D19:D20"/>
@@ -5164,9 +5173,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="8" width="21.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.44140625" collapsed="true"/>
+    <col min="3" max="8" customWidth="true" width="21.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -5207,7 +5216,7 @@
       </c>
       <c r="D2" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="E2" t="s">
         <v>71</v>
@@ -5234,7 +5243,7 @@
       </c>
       <c r="D3" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="E3" t="s">
         <v>71</v>
@@ -5261,7 +5270,7 @@
       </c>
       <c r="D4" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
@@ -5288,7 +5297,7 @@
       </c>
       <c r="D5" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="E5" t="s">
         <v>71</v>
@@ -5315,7 +5324,7 @@
       </c>
       <c r="D6" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="E6" t="s">
         <v>71</v>
@@ -5332,13 +5341,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4060209A-0B38-4661-9596-27A202D9FCC3}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4060209A-0B38-4661-9596-27A202D9FCC3}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
@@ -5346,7 +5355,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -5357,17 +5366,17 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>"r"&amp;'TC19- Sales Order No'!$A$2&amp;"-01"</f>
-        <v>rss1731-2310001-01</v>
+        <v>rss1735-2311001-01</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81805742-040D-4C75-AD7F-AC26A3786CA2}">
-  <dimension ref="A1:U6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81805742-040D-4C75-AD7F-AC26A3786CA2}">
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
@@ -5375,12 +5384,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="20" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.77734375" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="6" max="20" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="17.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -5678,20 +5687,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93B6DC3-11C4-484A-99A7-37E57C28C17F}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93B6DC3-11C4-484A-99A7-37E57C28C17F}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="7" width="24" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="2" max="7" customWidth="true" width="24.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -5713,54 +5724,54 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B2" s="33">
-        <v>800</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34">
-        <v>700</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="C2" s="33">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B3" s="33">
-        <v>1500</v>
-      </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33">
-        <v>1500</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="C3" s="33">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B4" s="33">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="33">
-        <v>1000</v>
-      </c>
-      <c r="D4" s="33"/>
+        <v>800</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34">
+        <v>700</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B5" s="33">
-        <v>1000</v>
-      </c>
-      <c r="C5" s="33">
-        <v>1000</v>
-      </c>
-      <c r="D5" s="33"/>
+        <v>1500</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33">
+        <v>1500</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -5777,22 +5788,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E6">
+    <sortCondition ref="A2:A6"/>
+  </sortState>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5330B2FD-88D7-4407-ACFA-FC66B38BF634}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5330B2FD-88D7-4407-ACFA-FC66B38BF634}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="31.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="8.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="3" customWidth="true" width="31.77734375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -5851,12 +5865,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5865,11 +5879,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="8" width="11.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="5" max="8" customWidth="true" width="11.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -5901,11 +5915,11 @@
       </c>
       <c r="B2" t="str">
         <f>"Sc17"&amp;"-"&amp;AutoIncrement!A2&amp;" "&amp;"Free"</f>
-        <v>Sc17-33 Free</v>
+        <v>Sc17-35 Free</v>
       </c>
       <c r="C2" t="str">
         <f>"Sc17"&amp;"-"&amp;AutoIncrement!A2&amp;" "&amp;"Free"&amp;"- 30 Days"</f>
-        <v>Sc17-33 Free- 30 Days</v>
+        <v>Sc17-35 Free- 30 Days</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -5921,12 +5935,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA414E7-A38B-4919-8C8F-D39CE665F9A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA414E7-A38B-4919-8C8F-D39CE665F9A5}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5935,11 +5949,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="7" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="4" max="7" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -6049,22 +6063,22 @@
       <c r="F6" s="31"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0E1383-5F8F-418A-8F6C-BD1F737AB025}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0E1383-5F8F-418A-8F6C-BD1F737AB025}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="21.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="3" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -6096,12 +6110,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC55F55F-CBAA-44C1-8C2F-96B3D03911C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC55F55F-CBAA-44C1-8C2F-96B3D03911C9}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6110,7 +6124,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="21.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="8" customWidth="true" width="21.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -6220,13 +6234,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1350DA43-153F-4D15-8B00-E8BA26878F38}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1350DA43-153F-4D15-8B00-E8BA26878F38}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -6234,7 +6248,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -6245,25 +6259,25 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>"r"&amp;'TC19- Sales Order No'!$A$2&amp;"-02"</f>
-        <v>rss1731-2310001-02</v>
+        <v>rss1735-2311001-02</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2925DC33-A3BF-4DC0-9998-0A8ED380A76F}">
-  <dimension ref="A1:U6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2925DC33-A3BF-4DC0-9998-0A8ED380A76F}">
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="96" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0" zoomScale="96">
       <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="21" width="30.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="21" customWidth="true" width="30.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -6557,26 +6571,26 @@
       <c r="S6" s="32"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0818C847-4211-4653-8825-BBEEDE381DD7}">
-  <dimension ref="A1:AE6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0818C847-4211-4653-8825-BBEEDE381DD7}">
+  <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="AA1" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
       <selection activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="20" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="21" max="31" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="7" max="20" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="21" max="31" customWidth="true" width="25.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
@@ -6941,13 +6955,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6FE45A-8ADD-4DCB-AC8A-544D349118A6}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6FE45A-8ADD-4DCB-AC8A-544D349118A6}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
@@ -6955,7 +6969,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -6965,35 +6979,35 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60525806-95C1-4FC3-A8EC-C8D201E4ADF4}">
-  <dimension ref="A1:Z7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60525806-95C1-4FC3-A8EC-C8D201E4ADF4}">
+  <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="20.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="39.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="19" width="20.77734375" customWidth="1" collapsed="1"/>
-    <col min="20" max="21" width="26.21875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="24" max="25" width="26.21875" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="24.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="39.6640625" collapsed="true"/>
+    <col min="7" max="19" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="20" max="21" customWidth="true" width="26.21875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="24" max="25" customWidth="true" width="26.21875" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="24.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
@@ -7085,14 +7099,14 @@
       </c>
       <c r="C2" t="str">
         <f>"o-PK-SUP-POC-230720001-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720001-33</v>
+        <v>o-PK-SUP-POC-230720001-35</v>
       </c>
       <c r="D2" s="30">
         <v>45218</v>
       </c>
       <c r="E2" t="str">
         <f>"B-230720001-"&amp;AutoIncrement!A2</f>
-        <v>B-230720001-33</v>
+        <v>B-230720001-35</v>
       </c>
       <c r="F2" t="s">
         <v>80</v>
@@ -7138,7 +7152,7 @@
       </c>
       <c r="T2" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="U2" t="s">
         <v>71</v>
@@ -7168,14 +7182,14 @@
       </c>
       <c r="C3" t="str">
         <f>"o-PK-SUP-POC-230720001-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720001-33</v>
+        <v>o-PK-SUP-POC-230720001-35</v>
       </c>
       <c r="D3" s="30">
         <v>45218</v>
       </c>
       <c r="E3" t="str">
         <f>"B-230720001-"&amp;AutoIncrement!A2</f>
-        <v>B-230720001-33</v>
+        <v>B-230720001-35</v>
       </c>
       <c r="F3" t="s">
         <v>83</v>
@@ -7221,7 +7235,7 @@
       </c>
       <c r="T3" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="U3" t="s">
         <v>71</v>
@@ -7251,14 +7265,14 @@
       </c>
       <c r="C4" t="str">
         <f>"o-PK-SUP-POC-230720001-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720001-33</v>
+        <v>o-PK-SUP-POC-230720001-35</v>
       </c>
       <c r="D4" s="30">
         <v>45218</v>
       </c>
       <c r="E4" t="str">
         <f>"B-230720001-"&amp;AutoIncrement!A2</f>
-        <v>B-230720001-33</v>
+        <v>B-230720001-35</v>
       </c>
       <c r="F4" t="s">
         <v>85</v>
@@ -7301,7 +7315,7 @@
       </c>
       <c r="T4" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="U4" t="s">
         <v>71</v>
@@ -7331,14 +7345,14 @@
       </c>
       <c r="C5" t="str">
         <f>"o-PK-SUP-POC-230720001-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720001-33</v>
+        <v>o-PK-SUP-POC-230720001-35</v>
       </c>
       <c r="D5" s="30">
         <v>45218</v>
       </c>
       <c r="E5" t="str">
         <f>"B-230720001-"&amp;AutoIncrement!A2</f>
-        <v>B-230720001-33</v>
+        <v>B-230720001-35</v>
       </c>
       <c r="F5" t="s">
         <v>87</v>
@@ -7381,7 +7395,7 @@
       </c>
       <c r="T5" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="U5" t="s">
         <v>71</v>
@@ -7411,7 +7425,7 @@
       </c>
       <c r="C6" t="str">
         <f>"o-PK-SUP-POC-230720002-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720002-33</v>
+        <v>o-PK-SUP-POC-230720002-35</v>
       </c>
       <c r="D6" s="30">
         <v>45218</v>
@@ -7457,7 +7471,7 @@
       </c>
       <c r="T6" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="U6" t="s">
         <v>71</v>
@@ -7487,7 +7501,7 @@
       </c>
       <c r="C7" t="str">
         <f>"o-PK-SUP-POC-230720002-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720002-33</v>
+        <v>o-PK-SUP-POC-230720002-35</v>
       </c>
       <c r="D7" s="30">
         <v>45218</v>
@@ -7533,7 +7547,7 @@
       </c>
       <c r="T7" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="U7" t="s">
         <v>71</v>
@@ -7556,14 +7570,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F725A8-76DA-4C31-ADD9-93AF9843AA91}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F725A8-76DA-4C31-ADD9-93AF9843AA91}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -7571,7 +7585,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -7588,13 +7602,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6652092F-6BEE-4175-A843-CC7A640F51D9}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6652092F-6BEE-4175-A843-CC7A640F51D9}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -7602,11 +7616,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="20.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="20.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -7650,13 +7664,172 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17D8D98-2282-4C9F-923F-9194E4B05AC4}">
-  <dimension ref="A1:Z2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17D8D98-2282-4C9F-923F-9194E4B05AC4}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="3" max="14" customWidth="true" width="16.21875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="16" max="26" customWidth="true" width="16.21875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="str">
+        <f>"S17_PKSUP-PKCUS"&amp;AutoIncrement!A2</f>
+        <v>S17_PKSUP-PKCUS35</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0</v>
+      </c>
+      <c r="R2" s="5">
+        <v>1</v>
+      </c>
+      <c r="S2" s="5">
+        <v>6</v>
+      </c>
+      <c r="T2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="U2" s="5">
+        <v>31</v>
+      </c>
+      <c r="V2" s="5">
+        <v>12</v>
+      </c>
+      <c r="W2" s="5">
+        <v>2024</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6596C3D8-DABB-4D68-A69F-3FC7822F2C01}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
@@ -7664,170 +7837,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="14" width="16.21875" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="16" max="26" width="16.21875" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="str">
-        <f>"S17_PKSUP-PKCUS"&amp;AutoIncrement!A2</f>
-        <v>S17_PKSUP-PKCUS33</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>0</v>
-      </c>
-      <c r="R2" s="5">
-        <v>1</v>
-      </c>
-      <c r="S2" s="5">
-        <v>6</v>
-      </c>
-      <c r="T2" s="5">
-        <v>2023</v>
-      </c>
-      <c r="U2" s="5">
-        <v>31</v>
-      </c>
-      <c r="V2" s="5">
-        <v>12</v>
-      </c>
-      <c r="W2" s="5">
-        <v>2024</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6596C3D8-DABB-4D68-A69F-3FC7822F2C01}">
-  <dimension ref="A1:M6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="8" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="13" width="44.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="4" max="8" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="9" max="13" customWidth="true" width="44.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -7946,13 +7960,13 @@
       <c r="F6" s="31"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433DDF3E-D550-4963-9030-F032BC0321D8}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433DDF3E-D550-4963-9030-F032BC0321D8}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -7960,7 +7974,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="24.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="5" customWidth="true" width="24.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -7998,13 +8012,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D46D62-1A05-4CC2-A672-78B90F2AFB42}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D46D62-1A05-4CC2-A672-78B90F2AFB42}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -8012,7 +8026,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -8023,17 +8037,17 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>"r"&amp;'TC19- Sales Order No'!$A$2&amp;"-03"</f>
-        <v>rss1731-2310001-03</v>
+        <v>rss1735-2311001-03</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632FFAE2-9695-4BBF-A4B6-845817944B45}">
-  <dimension ref="A1:V6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632FFAE2-9695-4BBF-A4B6-845817944B45}">
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView topLeftCell="Q2" workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
@@ -8041,10 +8055,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31" customWidth="1" collapsed="1"/>
-    <col min="3" max="21" width="21.77734375" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="23.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="3" max="21" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="23.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
@@ -8341,13 +8355,13 @@
       <c r="S6" s="32"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3919EC5C-738D-46A4-B507-DE2D70B89DAC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3919EC5C-738D-46A4-B507-DE2D70B89DAC}">
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -8356,7 +8370,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="22" width="32.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="22" customWidth="true" width="32.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -8640,12 +8654,12 @@
       <c r="R6" s="32"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E777727B-1DDD-4CFF-AA09-5D5BC85D3018}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E777727B-1DDD-4CFF-AA09-5D5BC85D3018}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8654,7 +8668,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="7" width="21" customWidth="1" collapsed="1"/>
+    <col min="2" max="7" customWidth="true" width="21.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -8746,13 +8760,13 @@
       <c r="E6" s="31"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58D9144-0E0B-49C9-886E-4A2CDDD2CEB0}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58D9144-0E0B-49C9-886E-4A2CDDD2CEB0}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
@@ -8760,7 +8774,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="31.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" width="31.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -8778,31 +8792,31 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="41">
+      <c r="A2" s="41" t="n">
         <f>'TC55- New Outbound Date'!A2</f>
-        <v>45244</v>
-      </c>
-      <c r="B2" s="41">
+        <v>45244.0</v>
+      </c>
+      <c r="B2" s="41" t="n">
         <f>'TC55- New Outbound Date'!B2</f>
-        <v>45247</v>
-      </c>
-      <c r="C2" s="41">
+        <v>45247.0</v>
+      </c>
+      <c r="C2" s="41" t="n">
         <f>'TC55- New Outbound Date'!C2</f>
-        <v>45257</v>
-      </c>
-      <c r="D2" s="40">
+        <v>45257.0</v>
+      </c>
+      <c r="D2" s="40" t="n">
         <f>'TC55- New Outbound Date'!D2</f>
-        <v>45301</v>
+        <v>45301.0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916ABB38-A115-43EF-A0AC-CEE6A4BC3E6C}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916ABB38-A115-43EF-A0AC-CEE6A4BC3E6C}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -8810,7 +8824,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -8821,17 +8835,17 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>"r"&amp;'TC19- Sales Order No'!$A$2&amp;"-04"</f>
-        <v>rss1731-2310001-04</v>
+        <v>rss1735-2311001-04</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798D413F-7C90-4167-9ECC-358646B148B3}">
-  <dimension ref="A1:AQ2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798D413F-7C90-4167-9ECC-358646B148B3}">
+  <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -8839,16 +8853,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="32" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="37" max="43" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="8" max="32" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="34" max="35" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="37" max="43" customWidth="true" width="14.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.3">
@@ -8982,14 +8996,14 @@
       </c>
       <c r="C2" t="str">
         <f>"o-PK-SUP-POC-230720003-"&amp;AutoIncrement!A2</f>
-        <v>o-PK-SUP-POC-230720003-33</v>
+        <v>o-PK-SUP-POC-230720003-35</v>
       </c>
       <c r="D2" s="30">
         <v>45218</v>
       </c>
       <c r="F2" t="str">
         <f>"B-230720001-"&amp;AutoIncrement!A2</f>
-        <v>B-230720001-33</v>
+        <v>B-230720001-35</v>
       </c>
       <c r="G2" t="s">
         <v>87</v>
@@ -9032,7 +9046,7 @@
       </c>
       <c r="AG2" t="str">
         <f>'TC19- Sales Order No'!$A$2</f>
-        <v>ss1731-2310001</v>
+        <v>ss1735-2311001</v>
       </c>
       <c r="AH2" t="s">
         <v>71</v>
@@ -9054,25 +9068,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A92A14-B736-4BE2-B5C8-4BD774DAC054}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A92A14-B736-4BE2-B5C8-4BD774DAC054}">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="41.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="23" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="41.109375" collapsed="true"/>
+    <col min="5" max="23" customWidth="true" width="25.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
@@ -9349,13 +9363,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A22F613-B9FC-4721-BAE7-2427DC0B0AB7}">
-  <dimension ref="A1:AE6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A22F613-B9FC-4721-BAE7-2427DC0B0AB7}">
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -9363,15 +9377,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="42" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="15.77734375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.77734375" customWidth="1" collapsed="1"/>
-    <col min="32" max="16384" width="8.88671875" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="32" max="16384" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -9421,7 +9435,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E2" s="13">
         <v>0.5</v>
@@ -9457,7 +9471,7 @@
       </c>
       <c r="D3" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E3" s="13">
         <v>0.5</v>
@@ -9493,7 +9507,7 @@
       </c>
       <c r="D4" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E4" s="13">
         <v>0.5</v>
@@ -9529,7 +9543,7 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E5" s="13">
         <v>0.5</v>
@@ -9553,7 +9567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="13.2" r="6" s="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>89</v>
       </c>
@@ -9565,7 +9579,7 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$B$2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="E6" s="14">
         <v>0.5</v>
@@ -9591,21 +9605,21 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3527525D-DCF3-42E0-8A83-320500061703}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3527525D-DCF3-42E0-8A83-320500061703}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="20.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -9617,46 +9631,49 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>219</v>
+      <c r="A2" t="str">
+        <f>'TC51- Outbound Details'!$E$2</f>
+        <v>B-230720001-35</v>
       </c>
       <c r="B2" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>219</v>
+      <c r="A3" t="str">
+        <f>'TC51- Outbound Details'!$E$2</f>
+        <v>B-230720001-35</v>
       </c>
       <c r="B3" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>219</v>
+      <c r="A4" t="str">
+        <f>'TC51- Outbound Details'!$E$2</f>
+        <v>B-230720001-35</v>
       </c>
       <c r="B4" t="s">
         <v>263</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07131E43-540D-4AB5-B799-C1C9E8C3480D}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07131E43-540D-4AB5-B799-C1C9E8C3480D}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -9724,13 +9741,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D61966F-68FA-4203-8F7A-1605789961DD}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D61966F-68FA-4203-8F7A-1605789961DD}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
@@ -9738,8 +9755,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -9753,38 +9770,38 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>'TC51- Outbound Details'!$C$2</f>
-        <v>o-PK-SUP-POC-230720001-33</v>
+        <v>o-PK-SUP-POC-230720001-35</v>
       </c>
       <c r="B2" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>'TC51- Outbound Details'!$C$6</f>
-        <v>o-PK-SUP-POC-230720002-33</v>
+        <v>o-PK-SUP-POC-230720002-35</v>
       </c>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>'TC69- Outbound Details'!$C$2</f>
-        <v>o-PK-SUP-POC-230720003-33</v>
+        <v>o-PK-SUP-POC-230720003-35</v>
       </c>
       <c r="B4" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256B465A-06B6-4028-A3DE-171E9F4E873E}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256B465A-06B6-4028-A3DE-171E9F4E873E}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
@@ -9792,8 +9809,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -9813,12 +9830,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813C15B5-BFA5-453B-8BB1-2BD28A10985D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813C15B5-BFA5-453B-8BB1-2BD28A10985D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9827,9 +9844,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="5" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -9873,12 +9890,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40266E76-E31A-42AB-9082-4A7187A8DFDB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40266E76-E31A-42AB-9082-4A7187A8DFDB}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9887,9 +9904,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="30.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="9.21875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="30.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -9909,10 +9926,10 @@
       </c>
       <c r="B2" t="str">
         <f>'TC75- Outbound Nos'!$B$2</f>
-        <v>o-PK-SUP-POC-231030001</v>
+        <v>o-PK-SUP-POC-231106001</v>
       </c>
       <c r="C2" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -9921,10 +9938,10 @@
       </c>
       <c r="B3" t="str">
         <f>'TC75- Outbound Nos'!$B$3</f>
-        <v>o-PK-SUP-POC-231030002</v>
+        <v>o-PK-SUP-POC-231106002</v>
       </c>
       <c r="C3" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -9933,22 +9950,22 @@
       </c>
       <c r="B4" t="str">
         <f>'TC75- Outbound Nos'!$B$4</f>
-        <v>o-PK-SUP-POC-231031001</v>
+        <v>o-PK-SUP-POC-231106003</v>
       </c>
       <c r="C4" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66A75C4-CFB3-461E-9746-0710E05709C6}">
-  <dimension ref="A1:V6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66A75C4-CFB3-461E-9746-0710E05709C6}">
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -9956,17 +9973,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="11" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.33203125" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="18" width="17.44140625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="37.6640625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="4" max="11" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.33203125" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="18" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="13.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
@@ -10043,7 +10060,7 @@
       </c>
       <c r="B2" s="6" t="str">
         <f>"PKSUPTOPKCUS17001-"&amp;'TC2- ReceivedRequestAddNewPart'!K2&amp;"-0"&amp;AutoIncrement!A2</f>
-        <v>PKSUPTOPKCUS17001-s1733-033</v>
+        <v>PKSUPTOPKCUS17001-s1735-035</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>72</v>
@@ -10071,7 +10088,7 @@
       </c>
       <c r="K2" s="18" t="str">
         <f>"s17"&amp;AutoIncrement!A2</f>
-        <v>s1733</v>
+        <v>s1735</v>
       </c>
       <c r="L2" t="s">
         <v>340</v>
@@ -10087,7 +10104,7 @@
       </c>
       <c r="R2" t="str">
         <f>'TC1-Description'!$A$2</f>
-        <v>s1733</v>
+        <v>s1735</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>341</v>
@@ -10100,22 +10117,22 @@
       <c r="B6" s="53"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736BFDB1-9F80-4554-8F12-819F55F4808D}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736BFDB1-9F80-4554-8F12-819F55F4808D}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -10129,37 +10146,37 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>'TC2- ReceivedRequestAddNewPart'!$K$2</f>
-        <v>s1733</v>
+        <v>s1735</v>
       </c>
       <c r="B2" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95ACEB6C-D089-4254-844E-E707AAF69C74}">
-  <dimension ref="A1:AC6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95ACEB6C-D089-4254-844E-E707AAF69C74}">
+  <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="45.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="17" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="33.21875" collapsed="true"/>
+    <col min="2" max="5" customWidth="true" width="45.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.44140625" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="16.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
@@ -10281,7 +10298,7 @@
       </c>
       <c r="J2" s="49" t="str">
         <f ca="1">TEXT(TODAY(), "mmm d, yyyy")</f>
-        <v>Nov 5, 2023</v>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R2">
         <v>10</v>
@@ -10349,8 +10366,8 @@
         <v>8</v>
       </c>
       <c r="J3" s="49" t="str">
-        <f t="shared" ref="J3:J6" ca="1" si="0">TEXT(TODAY(), "mmm d, yyyy")</f>
-        <v>Nov 5, 2023</v>
+        <f ca="1" ref="J3:J6" si="0" t="shared">TEXT(TODAY(), "mmm d, yyyy")</f>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R3">
         <v>10</v>
@@ -10418,8 +10435,8 @@
         <v>10</v>
       </c>
       <c r="J4" s="49" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Nov 5, 2023</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R4">
         <v>10</v>
@@ -10487,8 +10504,8 @@
         <v>10</v>
       </c>
       <c r="J5" s="49" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Nov 5, 2023</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R5">
         <v>10</v>
@@ -10556,8 +10573,8 @@
         <v>101</v>
       </c>
       <c r="J6" s="49" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Nov 5, 2023</v>
+        <f ca="1" si="0" t="shared"/>
+        <v>Nov 6, 2023</v>
       </c>
       <c r="R6">
         <v>10</v>
@@ -10598,6 +10615,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>